<commit_message>
Updated mapping sheet with delete nodes
</commit_message>
<xml_diff>
--- a/schemas/Warrant_iepd/artifacts/Warrant_MappingSpreadsheet.xlsx
+++ b/schemas/Warrant_iepd/artifacts/Warrant_MappingSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28605"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\BL6PEPF0002A661\EXCELCNV\34b64021-a70c-4d84-8abd-ab5c3f7c7c9e\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay\Documents\IEPD\JTMP-Data-Exchange-Specs\schemas\Warrant_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="532" documentId="8_{1CA70B20-EC04-46B6-AFE0-7E9E1AC638AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66A76E70-075C-479B-B1A9-663ABF3F3669}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6E3A2F-0DE0-445F-8B27-37D70C0A3F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="19380" windowHeight="20970" tabRatio="781" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1809" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="897">
   <si>
     <t xml:space="preserve">Template last updated: </t>
   </si>
@@ -3363,6 +3363,242 @@
   </si>
   <si>
     <t xml:space="preserve">Literal </t>
+  </si>
+  <si>
+    <t>j:CourtOrderIssuingDate</t>
+  </si>
+  <si>
+    <t>delete nc:Date</t>
+  </si>
+  <si>
+    <t>j:CourtOrderStatus</t>
+  </si>
+  <si>
+    <t>delete nc:StatusDescriptionText</t>
+  </si>
+  <si>
+    <t>nc:Case</t>
+  </si>
+  <si>
+    <t>delete nc:ActivityLocation</t>
+  </si>
+  <si>
+    <t>j:Warrant</t>
+  </si>
+  <si>
+    <t>delete extra scr:WarrantAugmentation</t>
+  </si>
+  <si>
+    <t>delete extra nola-ext:WarrantAugmentation</t>
+  </si>
+  <si>
+    <t>j:ChargeFilingDate</t>
+  </si>
+  <si>
+    <t>nola-ext:WarrantServiceAttempt/j:CourtOrderServiceDate</t>
+  </si>
+  <si>
+    <t>nc:ActivityLocation</t>
+  </si>
+  <si>
+    <t>delete extra nc:Address</t>
+  </si>
+  <si>
+    <t>delete extra nc:CrossStreetAddress</t>
+  </si>
+  <si>
+    <t>nc:ActivityLocation/nc:Address</t>
+  </si>
+  <si>
+    <t>nola-ext:WarrantServiceAttempt/nc:Address</t>
+  </si>
+  <si>
+    <t>delete extra nc:AddressDeliveryPointID</t>
+  </si>
+  <si>
+    <t>delete extra nc:AddressStreet</t>
+  </si>
+  <si>
+    <t>nc:ActivityLocation/nc:Address/nc:AddressState</t>
+  </si>
+  <si>
+    <t>nola-ext:WarrantServiceAttempt/nc:Address/nc:AddressState</t>
+  </si>
+  <si>
+    <t>delete extra nc:StateName</t>
+  </si>
+  <si>
+    <t>delete extra ncic:StateUSCode</t>
+  </si>
+  <si>
+    <t>j:CourtOrderIssuingCourt</t>
+  </si>
+  <si>
+    <t>delete j:OrganizationAugmentation</t>
+  </si>
+  <si>
+    <t>delete nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>j:CourtOrderServiceOfficialEnforcement/nola-ext:PersonAugmentation/nc:PersonEmploymentAssociation/nc:Employer</t>
+  </si>
+  <si>
+    <t>delete both hs:EmployerAugmentation</t>
+  </si>
+  <si>
+    <t>delete both nola-ext:EmployerAugmentation</t>
+  </si>
+  <si>
+    <t>delete both EntityPerson</t>
+  </si>
+  <si>
+    <t>delete extra nc:EntityOrganization</t>
+  </si>
+  <si>
+    <t>j:CourtOrderServiceOfficialEnforcement/nola-ext:PersonAugmentation/nc:PersonEmploymentAssociation</t>
+  </si>
+  <si>
+    <t>delete j:EnforcementOfficialBadgeIdentification</t>
+  </si>
+  <si>
+    <t>j:CourtOrderServiceOfficialEnforcement/nc:RoleOfPerson</t>
+  </si>
+  <si>
+    <t>delete nc:PersonBirthDate</t>
+  </si>
+  <si>
+    <t>delete ncic:PersonEyeColorCode</t>
+  </si>
+  <si>
+    <t>delete ncic:PersonHairColorCode</t>
+  </si>
+  <si>
+    <t>delete nc:PersonHeightDescriptionText</t>
+  </si>
+  <si>
+    <t>delete nc:PersonHeightMeasure</t>
+  </si>
+  <si>
+    <t>delete ncic:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>delete ncic:PersonSexCode</t>
+  </si>
+  <si>
+    <t>delete nc:PersonSSNIdentification</t>
+  </si>
+  <si>
+    <t>delete nc:PersonStateIdentification</t>
+  </si>
+  <si>
+    <t>delete nc:PersonUSCitizenIndicator</t>
+  </si>
+  <si>
+    <t>delete nc:PersonWeightDescriptionText</t>
+  </si>
+  <si>
+    <t>delete nc:PersonWeightMeasure</t>
+  </si>
+  <si>
+    <t>delete nc:PersonContactInformation</t>
+  </si>
+  <si>
+    <t>j:CourtOrderServiceOfficialEnforcement/nc:RoleOfPerson/nc:PersonName</t>
+  </si>
+  <si>
+    <t>delete nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>delete nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>delete nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>delete nc:PersonNameSuffixText</t>
+  </si>
+  <si>
+    <t>j:CourtOrderRequestEntity/nc:EntityPerson</t>
+  </si>
+  <si>
+    <t>j:CourtOrderRequestEntity/nc:EntityPerson/nc:PersonName</t>
+  </si>
+  <si>
+    <t>j:CourtOrderRequestEntity</t>
+  </si>
+  <si>
+    <t>j:CourtOrderRequestEntity/nc:EntityPerson/nola-ext:PersonAugmentation/nc:PersonEmploymentAssociation/nc:Employer</t>
+  </si>
+  <si>
+    <t>If missing add
+&lt;nc:EntityOrganization&gt;
+                                &lt;nc:OrganizationIdentification&gt;
+                                    &lt;nc:IdentificationID&gt;string&lt;/nc:IdentificationID&gt;
+                                &lt;/nc:OrganizationIdentification&gt;
+                                &lt;nc:OrganizationName&gt;string&lt;/nc:OrganizationName&gt;
+                                &lt;j:OrganizationAugmentation&gt;
+                                    &lt;j:OrganizationORIIdentification&gt;
+                                        &lt;nc:IdentificationID&gt;string&lt;/nc:IdentificationID&gt;
+                                    &lt;/j:OrganizationORIIdentification&gt;
+                                &lt;/j:OrganizationAugmentation&gt;
+                            &lt;/nc:EntityOrganization&gt;</t>
+  </si>
+  <si>
+    <t>j:CourtOrderIssuingJudicialOfficial/nc:RoleOfPerson</t>
+  </si>
+  <si>
+    <t>nola-ext:PersonAugmentation</t>
+  </si>
+  <si>
+    <t>j:CourtOrderIssuingJudicialOfficial/nc:RoleOfPerson/nc:PersonName</t>
+  </si>
+  <si>
+    <t>j:CourtOrderDesignatedSubject/nc:RoleOfPerson/nc:PersonBirthDate</t>
+  </si>
+  <si>
+    <t>delete nc:DateTime</t>
+  </si>
+  <si>
+    <t>j:CourtOrderDesignatedSubject/nc:RoleOfPerson/nc:PersonName</t>
+  </si>
+  <si>
+    <t>delete nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>j:CourtOrderDesignatedSubject/nc:RoleOfPerson/nc:PersonContactInformation</t>
+  </si>
+  <si>
+    <t>delete extra nc:ContactTelephoneNumber</t>
+  </si>
+  <si>
+    <t>delete extra nc:ContactMailingAddress</t>
+  </si>
+  <si>
+    <t>j:CourtOrderDesignatedSubject/nc:RoleOfPerson/nc:PersonContactInformation/nc:Address</t>
+  </si>
+  <si>
+    <t>j:CourtOrderDesignatedSubject/nc:RoleOfPerson/nc:PersonContactInformation/nc:Address/nc:AddressState</t>
+  </si>
+  <si>
+    <t>j:CourtOrderDesignatedSubject/nc:RoleOfPerson/nola-ext:PersonAugmentation/nc:PersonEmploymentAssociation/nc:Employer</t>
+  </si>
+  <si>
+    <t>delete extra nola-ext:EmployerAugmentation</t>
+  </si>
+  <si>
+    <t>delete extra hs:EmployerAugmentation</t>
+  </si>
+  <si>
+    <t>delete both nc:EntityPerson</t>
+  </si>
+  <si>
+    <t>delete nc:EntityOrganization</t>
+  </si>
+  <si>
+    <t>j:CourtOrderDesignatedSubject/nc:RoleOfPerson/nola-ext:PersonAugmentation/nc:PersonEmploymentAssociation/nc:Employer/nola-ext:EmployerAugmentation</t>
+  </si>
+  <si>
+    <t>delete nc:StatusText</t>
   </si>
 </sst>
 </file>
@@ -3777,16 +4013,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
         <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -3863,7 +4095,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4150,20 +4382,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="71">
@@ -5850,10 +6088,10 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="51.453125" style="17" customWidth="1"/>
     <col min="3" max="4" width="35" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5879,7 +6117,7 @@
       <c r="A4" s="28"/>
       <c r="B4" s="28"/>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="29">
       <c r="A5" s="29" t="s">
         <v>3</v>
       </c>
@@ -5935,7 +6173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30">
+    <row r="9" spans="1:4">
       <c r="A9" s="30" t="s">
         <v>18</v>
       </c>
@@ -5949,7 +6187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30">
+    <row r="10" spans="1:4" ht="29">
       <c r="A10" s="30" t="s">
         <v>21</v>
       </c>
@@ -6022,7 +6260,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30">
+    <row r="18" spans="1:4" ht="29">
       <c r="A18" s="29" t="s">
         <v>36</v>
       </c>
@@ -6036,7 +6274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45">
+    <row r="19" spans="1:4" ht="43.5">
       <c r="A19" s="31" t="s">
         <v>37</v>
       </c>
@@ -6050,7 +6288,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="60">
+    <row r="20" spans="1:4" ht="43.5">
       <c r="A20" s="31" t="s">
         <v>41</v>
       </c>
@@ -6064,7 +6302,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45">
+    <row r="21" spans="1:4" ht="43.5">
       <c r="A21" s="31" t="s">
         <v>45</v>
       </c>
@@ -6078,7 +6316,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45">
+    <row r="22" spans="1:4" ht="29">
       <c r="A22" s="31" t="s">
         <v>49</v>
       </c>
@@ -6092,7 +6330,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30">
+    <row r="23" spans="1:4" ht="29">
       <c r="A23" s="31" t="s">
         <v>52</v>
       </c>
@@ -6106,7 +6344,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="45">
+    <row r="24" spans="1:4" ht="43.5">
       <c r="A24" s="31" t="s">
         <v>56</v>
       </c>
@@ -6120,7 +6358,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="60">
+    <row r="25" spans="1:4" ht="43.5">
       <c r="A25" s="31" t="s">
         <v>60</v>
       </c>
@@ -6134,7 +6372,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="45">
+    <row r="26" spans="1:4" ht="43.5">
       <c r="A26" s="31" t="s">
         <v>63</v>
       </c>
@@ -6148,7 +6386,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="90">
+    <row r="27" spans="1:4" ht="87">
       <c r="A27" s="31" t="s">
         <v>67</v>
       </c>
@@ -6162,7 +6400,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="45">
+    <row r="28" spans="1:4" ht="43.5">
       <c r="A28" s="31" t="s">
         <v>71</v>
       </c>
@@ -6184,7 +6422,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="90">
+    <row r="32" spans="1:4" ht="72.5">
       <c r="A32" s="5" t="s">
         <v>76</v>
       </c>
@@ -6192,7 +6430,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="60">
+    <row r="33" spans="1:2" ht="58">
       <c r="A33" s="5" t="s">
         <v>78</v>
       </c>
@@ -6200,7 +6438,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="45">
+    <row r="34" spans="1:2" ht="43.5">
       <c r="A34" s="5" t="s">
         <v>80</v>
       </c>
@@ -6208,7 +6446,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="30">
+    <row r="35" spans="1:2" ht="29">
       <c r="A35" s="5" t="s">
         <v>82</v>
       </c>
@@ -6216,7 +6454,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="45">
+    <row r="36" spans="1:2" ht="43.5">
       <c r="A36" s="5" t="s">
         <v>84</v>
       </c>
@@ -6224,7 +6462,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="30">
+    <row r="37" spans="1:2" ht="29">
       <c r="A37" s="5" t="s">
         <v>86</v>
       </c>
@@ -6232,7 +6470,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="30">
+    <row r="38" spans="1:2" ht="29">
       <c r="A38" s="5" t="s">
         <v>88</v>
       </c>
@@ -6240,7 +6478,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="105">
+    <row r="39" spans="1:2" ht="101.5">
       <c r="A39" s="30" t="s">
         <v>90</v>
       </c>
@@ -6248,7 +6486,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="90">
+    <row r="40" spans="1:2" ht="72.5">
       <c r="A40" s="30" t="s">
         <v>92</v>
       </c>
@@ -6275,21 +6513,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="2" customWidth="1"/>
-    <col min="2" max="4" width="20.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="17" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="17" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="30.42578125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="15.453125" style="2" customWidth="1"/>
+    <col min="2" max="4" width="20.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" style="17" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" style="17" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="23.81640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="30.453125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30">
+    <row r="1" spans="1:11" ht="29">
       <c r="A1" s="10" t="s">
         <v>819</v>
       </c>
@@ -6347,13 +6585,13 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="3.453125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" style="17" customWidth="1"/>
     <col min="3" max="3" width="76" style="17" customWidth="1"/>
-    <col min="4" max="5" width="29.42578125" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="16"/>
+    <col min="4" max="5" width="29.453125" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -6415,7 +6653,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="29">
       <c r="A10" s="68"/>
       <c r="B10" s="69" t="s">
         <v>105</v>
@@ -6465,7 +6703,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30">
+    <row r="16" spans="1:3" ht="29">
       <c r="A16" s="68"/>
       <c r="B16" s="70" t="s">
         <v>115</v>
@@ -6483,7 +6721,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" s="68"/>
       <c r="B18" s="70" t="s">
         <v>119</v>
@@ -6578,7 +6816,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30">
+    <row r="29" spans="1:3" ht="29">
       <c r="A29" s="68"/>
       <c r="B29" s="69" t="s">
         <v>10</v>
@@ -6596,7 +6834,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30">
+    <row r="31" spans="1:3" ht="29">
       <c r="A31" s="68"/>
       <c r="B31" s="69" t="s">
         <v>105</v>
@@ -6709,7 +6947,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="30">
+    <row r="46" spans="1:3" ht="29">
       <c r="A46" s="42"/>
       <c r="B46" s="32" t="s">
         <v>152</v>
@@ -6727,7 +6965,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="60">
+    <row r="48" spans="1:3" ht="58">
       <c r="A48" s="42"/>
       <c r="B48" s="32" t="s">
         <v>154</v>
@@ -6743,7 +6981,7 @@
       </c>
       <c r="C49" s="43"/>
     </row>
-    <row r="50" spans="1:3" ht="30">
+    <row r="50" spans="1:3" ht="29">
       <c r="A50" s="42"/>
       <c r="B50" s="49" t="s">
         <v>157</v>
@@ -6770,7 +7008,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="30">
+    <row r="53" spans="1:3" ht="29">
       <c r="A53" s="42"/>
       <c r="B53" s="32" t="s">
         <v>163</v>
@@ -6813,7 +7051,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="30">
+    <row r="58" spans="1:3" ht="29">
       <c r="A58" s="8"/>
       <c r="B58" s="7" t="s">
         <v>172</v>
@@ -6822,7 +7060,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="30">
+    <row r="59" spans="1:3" ht="29">
       <c r="A59" s="8"/>
       <c r="B59" s="7" t="s">
         <v>174</v>
@@ -6831,7 +7069,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="30">
+    <row r="60" spans="1:3" ht="29">
       <c r="A60" s="8"/>
       <c r="B60" s="7" t="s">
         <v>176</v>
@@ -6840,7 +7078,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="30">
+    <row r="61" spans="1:3" ht="29">
       <c r="A61" s="8"/>
       <c r="B61" s="7" t="s">
         <v>178</v>
@@ -6998,7 +7236,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="30">
+    <row r="81" spans="1:3" ht="29">
       <c r="A81" s="40"/>
       <c r="B81" s="49" t="s">
         <v>193</v>
@@ -7043,7 +7281,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="30">
+    <row r="86" spans="1:3" ht="29">
       <c r="A86" s="40"/>
       <c r="B86" s="49" t="s">
         <v>203</v>
@@ -7052,7 +7290,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="30">
+    <row r="87" spans="1:3" ht="29">
       <c r="A87" s="40"/>
       <c r="B87" s="49" t="s">
         <v>205</v>
@@ -7061,7 +7299,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="45">
+    <row r="88" spans="1:3" ht="29">
       <c r="A88" s="40"/>
       <c r="B88" s="32" t="s">
         <v>207</v>
@@ -7070,7 +7308,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="75">
+    <row r="89" spans="1:3" ht="72.5">
       <c r="A89" s="40"/>
       <c r="B89" s="32" t="s">
         <v>209</v>
@@ -7079,7 +7317,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="75" hidden="1">
+    <row r="90" spans="1:3" ht="72.5" hidden="1">
       <c r="A90" s="40"/>
       <c r="B90" s="32" t="s">
         <v>211</v>
@@ -7104,7 +7342,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="30">
+    <row r="93" spans="1:3" ht="29">
       <c r="A93" s="8"/>
       <c r="B93" s="7" t="s">
         <v>214</v>
@@ -7113,7 +7351,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="30">
+    <row r="94" spans="1:3" ht="29">
       <c r="A94" s="8"/>
       <c r="B94" s="7" t="s">
         <v>216</v>
@@ -7187,7 +7425,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="30">
+    <row r="104" spans="1:3">
       <c r="A104" s="39"/>
       <c r="B104" s="32" t="s">
         <v>223</v>
@@ -7196,7 +7434,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="45">
+    <row r="105" spans="1:3" ht="29">
       <c r="A105" s="39"/>
       <c r="B105" s="32" t="s">
         <v>225</v>
@@ -7264,7 +7502,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="113" spans="1:3" customFormat="1" ht="30">
+    <row r="113" spans="1:3" customFormat="1">
       <c r="A113" s="39"/>
       <c r="B113" s="32" t="s">
         <v>223</v>
@@ -7282,7 +7520,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="30">
+    <row r="115" spans="1:3">
       <c r="A115" s="39"/>
       <c r="B115" s="32" t="s">
         <v>225</v>
@@ -7448,7 +7686,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="30">
+    <row r="137" spans="1:3" ht="29">
       <c r="A137" s="40"/>
       <c r="B137" s="32" t="s">
         <v>242</v>
@@ -7721,7 +7959,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="30">
+    <row r="170" spans="1:3" ht="29">
       <c r="A170" s="40"/>
       <c r="B170" s="49" t="s">
         <v>283</v>
@@ -7766,7 +8004,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="30">
+    <row r="175" spans="1:3" ht="29">
       <c r="A175" s="40"/>
       <c r="B175" s="49" t="s">
         <v>293</v>
@@ -7775,7 +8013,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="30">
+    <row r="176" spans="1:3" ht="29">
       <c r="A176" s="40"/>
       <c r="B176" s="49" t="s">
         <v>295</v>
@@ -7895,7 +8133,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="30">
+    <row r="193" spans="1:3">
       <c r="A193" s="39"/>
       <c r="B193" s="32" t="s">
         <v>313</v>
@@ -7954,7 +8192,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="30">
+    <row r="200" spans="1:3">
       <c r="A200" s="40"/>
       <c r="B200" s="32" t="s">
         <v>313</v>
@@ -8030,11 +8268,11 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="86.42578125" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="24.1796875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="86.453125" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
@@ -8060,7 +8298,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.35" customHeight="1">
+    <row r="6" spans="1:2" ht="43.4" customHeight="1">
       <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
@@ -8098,7 +8336,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="43.35" customHeight="1">
+    <row r="15" spans="1:2" ht="43.4" customHeight="1">
       <c r="A15" s="20" t="s">
         <v>4</v>
       </c>
@@ -8126,7 +8364,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="43.35" customHeight="1">
+    <row r="22" spans="1:2" ht="43.4" customHeight="1">
       <c r="A22" s="20" t="s">
         <v>4</v>
       </c>
@@ -8181,45 +8419,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC308"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+    <sheetView zoomScale="133" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="N28" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="O29" sqref="O29"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="52.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="43.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.26953125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" style="2" customWidth="1"/>
     <col min="9" max="9" width="50" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="46.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="37.7109375" style="2" customWidth="1"/>
-    <col min="13" max="14" width="12.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="46.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.81640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="37.7265625" style="2" customWidth="1"/>
+    <col min="13" max="14" width="12.453125" style="2" customWidth="1"/>
     <col min="15" max="15" width="79" style="2" customWidth="1"/>
-    <col min="16" max="16" width="34.140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="23.28515625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="85.5703125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.42578125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="31.42578125" style="2" customWidth="1"/>
-    <col min="24" max="25" width="31.85546875" style="2" customWidth="1"/>
-    <col min="26" max="26" width="26.42578125" style="2" customWidth="1"/>
-    <col min="27" max="27" width="9.140625" style="2"/>
-    <col min="28" max="28" width="77.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="2"/>
+    <col min="16" max="16" width="34.1796875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="23.26953125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="14.453125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="85.54296875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.453125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="17.453125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="31.453125" style="2" customWidth="1"/>
+    <col min="24" max="25" width="31.81640625" style="2" customWidth="1"/>
+    <col min="26" max="26" width="26.453125" style="2" customWidth="1"/>
+    <col min="27" max="27" width="9.1796875" style="2"/>
+    <col min="28" max="28" width="77.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="56" customFormat="1" ht="30.75">
+    <row r="1" spans="1:29" s="56" customFormat="1" ht="29.5">
       <c r="A1" s="3" t="s">
         <v>325</v>
       </c>
@@ -8297,7 +8535,7 @@
       </c>
       <c r="AC1" s="88"/>
     </row>
-    <row r="2" spans="1:29" ht="80.45" customHeight="1">
+    <row r="2" spans="1:29" ht="80.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>343</v>
       </c>
@@ -8387,7 +8625,7 @@
       </c>
       <c r="AC3" s="88"/>
     </row>
-    <row r="4" spans="1:29" ht="30.75">
+    <row r="4" spans="1:29" ht="16">
       <c r="B4" t="s">
         <v>364</v>
       </c>
@@ -8422,7 +8660,7 @@
       </c>
       <c r="AC4" s="94"/>
     </row>
-    <row r="5" spans="1:29" ht="30.75">
+    <row r="5" spans="1:29" ht="29.5">
       <c r="A5" s="2" t="s">
         <v>370</v>
       </c>
@@ -8467,7 +8705,7 @@
       </c>
       <c r="AC5" s="88"/>
     </row>
-    <row r="6" spans="1:29" ht="45.75">
+    <row r="6" spans="1:29" ht="44">
       <c r="A6" s="2" t="s">
         <v>343</v>
       </c>
@@ -8509,7 +8747,7 @@
       </c>
       <c r="AC6" s="88"/>
     </row>
-    <row r="7" spans="1:29" ht="60.75">
+    <row r="7" spans="1:29" ht="29.5">
       <c r="A7" s="2" t="s">
         <v>370</v>
       </c>
@@ -8554,7 +8792,7 @@
       </c>
       <c r="AC7" s="94"/>
     </row>
-    <row r="8" spans="1:29" ht="60.75">
+    <row r="8" spans="1:29" ht="29.5">
       <c r="A8" s="2" t="s">
         <v>370</v>
       </c>
@@ -8599,7 +8837,7 @@
       </c>
       <c r="AC8" s="94"/>
     </row>
-    <row r="9" spans="1:29" ht="45.75">
+    <row r="9" spans="1:29" ht="44">
       <c r="A9" s="2" t="s">
         <v>343</v>
       </c>
@@ -8644,7 +8882,7 @@
       </c>
       <c r="AC9" s="88"/>
     </row>
-    <row r="10" spans="1:29" ht="91.5">
+    <row r="10" spans="1:29" ht="87.5">
       <c r="A10" s="2" t="s">
         <v>370</v>
       </c>
@@ -8689,7 +8927,7 @@
       </c>
       <c r="AC10" s="88"/>
     </row>
-    <row r="11" spans="1:29" ht="60.75">
+    <row r="11" spans="1:29" ht="29.5">
       <c r="A11" s="2" t="s">
         <v>410</v>
       </c>
@@ -8734,7 +8972,7 @@
       </c>
       <c r="AC11" s="88"/>
     </row>
-    <row r="12" spans="1:29" ht="60.75">
+    <row r="12" spans="1:29" ht="29.5">
       <c r="A12" s="2" t="s">
         <v>410</v>
       </c>
@@ -8775,7 +9013,7 @@
       </c>
       <c r="AC12" s="88"/>
     </row>
-    <row r="13" spans="1:29" ht="60.75">
+    <row r="13" spans="1:29" ht="29.5">
       <c r="A13" s="2" t="s">
         <v>410</v>
       </c>
@@ -8816,7 +9054,7 @@
       </c>
       <c r="AC13" s="88"/>
     </row>
-    <row r="14" spans="1:29" ht="60.75">
+    <row r="14" spans="1:29" ht="29.5">
       <c r="A14" s="2" t="s">
         <v>410</v>
       </c>
@@ -8857,7 +9095,7 @@
       </c>
       <c r="AC14" s="88"/>
     </row>
-    <row r="15" spans="1:29" ht="60.75">
+    <row r="15" spans="1:29" ht="44">
       <c r="A15" s="2" t="s">
         <v>410</v>
       </c>
@@ -8905,7 +9143,7 @@
       </c>
       <c r="AC15" s="88"/>
     </row>
-    <row r="16" spans="1:29" ht="45.75">
+    <row r="16" spans="1:29" ht="29.5">
       <c r="A16" s="2" t="s">
         <v>410</v>
       </c>
@@ -8950,7 +9188,7 @@
       </c>
       <c r="AC16" s="88"/>
     </row>
-    <row r="17" spans="1:29" ht="60.75">
+    <row r="17" spans="1:29" ht="29.5">
       <c r="A17" s="2" t="s">
         <v>410</v>
       </c>
@@ -8995,7 +9233,7 @@
       </c>
       <c r="AC17" s="88"/>
     </row>
-    <row r="18" spans="1:29" ht="76.5">
+    <row r="18" spans="1:29" ht="29.5">
       <c r="B18" t="s">
         <v>456</v>
       </c>
@@ -9033,7 +9271,7 @@
       </c>
       <c r="AC18" s="88"/>
     </row>
-    <row r="19" spans="1:29" ht="60.75">
+    <row r="19" spans="1:29" ht="29.5">
       <c r="A19" s="2" t="s">
         <v>410</v>
       </c>
@@ -9078,7 +9316,7 @@
       </c>
       <c r="AC19" s="88"/>
     </row>
-    <row r="20" spans="1:29" ht="60.75">
+    <row r="20" spans="1:29" ht="29.5">
       <c r="A20" s="2" t="s">
         <v>410</v>
       </c>
@@ -9123,7 +9361,7 @@
       </c>
       <c r="AC20" s="88"/>
     </row>
-    <row r="21" spans="1:29" ht="60.75">
+    <row r="21" spans="1:29" ht="29.5">
       <c r="A21" s="2" t="s">
         <v>410</v>
       </c>
@@ -9168,7 +9406,7 @@
       </c>
       <c r="AC21" s="88"/>
     </row>
-    <row r="22" spans="1:29" ht="60.75">
+    <row r="22" spans="1:29" ht="29.5">
       <c r="A22" s="2" t="s">
         <v>410</v>
       </c>
@@ -9213,7 +9451,7 @@
       </c>
       <c r="AC22" s="88"/>
     </row>
-    <row r="23" spans="1:29" ht="76.5">
+    <row r="23" spans="1:29" ht="29.5">
       <c r="B23"/>
       <c r="C23" s="81"/>
       <c r="I23" s="84" t="s">
@@ -9249,7 +9487,7 @@
       </c>
       <c r="AC23" s="88"/>
     </row>
-    <row r="24" spans="1:29" ht="76.5">
+    <row r="24" spans="1:29" ht="44">
       <c r="A24" s="2" t="s">
         <v>410</v>
       </c>
@@ -9294,7 +9532,7 @@
       </c>
       <c r="AC24" s="88"/>
     </row>
-    <row r="25" spans="1:29" ht="76.5">
+    <row r="25" spans="1:29" ht="44">
       <c r="B25" t="s">
         <v>500</v>
       </c>
@@ -9334,7 +9572,7 @@
       </c>
       <c r="AC25" s="88"/>
     </row>
-    <row r="26" spans="1:29" ht="45.75">
+    <row r="26" spans="1:29" ht="29.5">
       <c r="B26" t="s">
         <v>505</v>
       </c>
@@ -9374,7 +9612,7 @@
       </c>
       <c r="AC26" s="88"/>
     </row>
-    <row r="27" spans="1:29" ht="60.75">
+    <row r="27" spans="1:29" ht="29.5">
       <c r="B27" t="s">
         <v>511</v>
       </c>
@@ -9414,7 +9652,7 @@
       </c>
       <c r="AC27" s="88"/>
     </row>
-    <row r="28" spans="1:29" ht="45.75">
+    <row r="28" spans="1:29" ht="44">
       <c r="B28" t="s">
         <v>518</v>
       </c>
@@ -9454,7 +9692,7 @@
       </c>
       <c r="AC28" s="88"/>
     </row>
-    <row r="29" spans="1:29" ht="45.75">
+    <row r="29" spans="1:29" ht="44">
       <c r="B29" s="105" t="s">
         <v>524</v>
       </c>
@@ -9494,7 +9732,7 @@
       </c>
       <c r="AC29" s="88"/>
     </row>
-    <row r="30" spans="1:29" ht="60.75">
+    <row r="30" spans="1:29" ht="29.5">
       <c r="A30" s="2" t="s">
         <v>410</v>
       </c>
@@ -9539,7 +9777,7 @@
       </c>
       <c r="AC30" s="88"/>
     </row>
-    <row r="31" spans="1:29" ht="60.75">
+    <row r="31" spans="1:29" ht="58.5">
       <c r="B31" t="s">
         <v>534</v>
       </c>
@@ -9583,7 +9821,7 @@
       </c>
       <c r="AC31" s="88"/>
     </row>
-    <row r="32" spans="1:29" ht="45.75">
+    <row r="32" spans="1:29" ht="29.5">
       <c r="B32" t="s">
         <v>540</v>
       </c>
@@ -9627,7 +9865,7 @@
       </c>
       <c r="AC32" s="88"/>
     </row>
-    <row r="33" spans="1:29" ht="45.75">
+    <row r="33" spans="1:29" ht="44">
       <c r="B33" t="s">
         <v>545</v>
       </c>
@@ -9671,7 +9909,7 @@
       </c>
       <c r="AC33" s="88"/>
     </row>
-    <row r="34" spans="1:29" s="103" customFormat="1" ht="45.75">
+    <row r="34" spans="1:29" s="103" customFormat="1" ht="16">
       <c r="A34" s="2"/>
       <c r="B34" t="s">
         <v>551</v>
@@ -9725,7 +9963,7 @@
       <c r="Y34" s="2"/>
       <c r="AC34" s="104"/>
     </row>
-    <row r="35" spans="1:29" ht="45.75">
+    <row r="35" spans="1:29" ht="16">
       <c r="B35" t="s">
         <v>556</v>
       </c>
@@ -9769,7 +10007,7 @@
       </c>
       <c r="AC35" s="88"/>
     </row>
-    <row r="36" spans="1:29" ht="45.75">
+    <row r="36" spans="1:29" ht="16">
       <c r="B36" t="s">
         <v>559</v>
       </c>
@@ -9822,7 +10060,7 @@
       <c r="Y36"/>
       <c r="AC36" s="88"/>
     </row>
-    <row r="37" spans="1:29" ht="45.75">
+    <row r="37" spans="1:29" ht="16">
       <c r="B37" t="s">
         <v>564</v>
       </c>
@@ -9875,7 +10113,7 @@
       <c r="Y37"/>
       <c r="AC37" s="88"/>
     </row>
-    <row r="38" spans="1:29" ht="30.75">
+    <row r="38" spans="1:29" ht="29.5">
       <c r="B38" t="s">
         <v>569</v>
       </c>
@@ -9928,7 +10166,7 @@
       <c r="Y38"/>
       <c r="AC38" s="88"/>
     </row>
-    <row r="39" spans="1:29" s="103" customFormat="1" ht="30.75">
+    <row r="39" spans="1:29" s="103" customFormat="1" ht="29.5">
       <c r="A39" s="2"/>
       <c r="B39" t="s">
         <v>574</v>
@@ -9982,7 +10220,7 @@
       <c r="Y39"/>
       <c r="AC39" s="104"/>
     </row>
-    <row r="40" spans="1:29" s="103" customFormat="1" ht="60.75">
+    <row r="40" spans="1:29" s="103" customFormat="1" ht="16">
       <c r="A40" s="2"/>
       <c r="B40" t="s">
         <v>577</v>
@@ -10036,7 +10274,7 @@
       <c r="Y40"/>
       <c r="AC40" s="104"/>
     </row>
-    <row r="41" spans="1:29" ht="45.75">
+    <row r="41" spans="1:29" ht="16">
       <c r="B41" t="s">
         <v>581</v>
       </c>
@@ -10089,7 +10327,7 @@
       <c r="Y41"/>
       <c r="AC41" s="88"/>
     </row>
-    <row r="42" spans="1:29" ht="45.75">
+    <row r="42" spans="1:29" ht="44">
       <c r="B42" t="s">
         <v>585</v>
       </c>
@@ -10142,7 +10380,7 @@
       <c r="Y42"/>
       <c r="AC42" s="88"/>
     </row>
-    <row r="43" spans="1:29" ht="45.75">
+    <row r="43" spans="1:29" ht="16">
       <c r="B43" t="s">
         <v>588</v>
       </c>
@@ -10285,7 +10523,7 @@
       <c r="Y45"/>
       <c r="AC45" s="88"/>
     </row>
-    <row r="46" spans="1:29" ht="30.75">
+    <row r="46" spans="1:29" ht="29.5">
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
@@ -10332,7 +10570,7 @@
       <c r="Y46" s="97"/>
       <c r="AC46" s="88"/>
     </row>
-    <row r="47" spans="1:29" ht="60.75">
+    <row r="47" spans="1:29" ht="16">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -10380,7 +10618,7 @@
       <c r="Y47" s="97"/>
       <c r="AC47" s="94"/>
     </row>
-    <row r="48" spans="1:29" ht="60.75">
+    <row r="48" spans="1:29" ht="29.5">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -10427,7 +10665,7 @@
       <c r="Y48" s="97"/>
       <c r="AC48" s="88"/>
     </row>
-    <row r="49" spans="1:29" ht="76.5">
+    <row r="49" spans="1:29" ht="58.5">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -10475,7 +10713,7 @@
       <c r="Y49" s="97"/>
       <c r="AC49" s="88"/>
     </row>
-    <row r="50" spans="1:29" ht="91.5">
+    <row r="50" spans="1:29" ht="29.5">
       <c r="A50" s="2" t="s">
         <v>410</v>
       </c>
@@ -10515,7 +10753,7 @@
       </c>
       <c r="AC50" s="88"/>
     </row>
-    <row r="51" spans="1:29" s="106" customFormat="1" ht="91.5">
+    <row r="51" spans="1:29" s="106" customFormat="1" ht="44">
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
@@ -10562,7 +10800,7 @@
       <c r="Y51"/>
       <c r="AC51" s="88"/>
     </row>
-    <row r="52" spans="1:29" s="106" customFormat="1" ht="91.5">
+    <row r="52" spans="1:29" s="106" customFormat="1" ht="44">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -10610,7 +10848,7 @@
       <c r="Y52"/>
       <c r="AC52" s="88"/>
     </row>
-    <row r="53" spans="1:29" ht="91.5">
+    <row r="53" spans="1:29" ht="29.5">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
@@ -10658,7 +10896,7 @@
       <c r="Y53"/>
       <c r="AC53" s="88"/>
     </row>
-    <row r="54" spans="1:29" ht="91.5">
+    <row r="54" spans="1:29" ht="29.5">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -10706,7 +10944,7 @@
       <c r="Y54"/>
       <c r="AC54" s="88"/>
     </row>
-    <row r="55" spans="1:29" ht="91.5">
+    <row r="55" spans="1:29" ht="29.5">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -10752,7 +10990,7 @@
       <c r="Y55"/>
       <c r="AC55" s="88"/>
     </row>
-    <row r="56" spans="1:29" ht="91.5">
+    <row r="56" spans="1:29" ht="44">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
@@ -10798,7 +11036,7 @@
       <c r="Y56"/>
       <c r="AC56" s="88"/>
     </row>
-    <row r="57" spans="1:29" ht="91.5">
+    <row r="57" spans="1:29" ht="29.5">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
@@ -10844,7 +11082,7 @@
       <c r="Y57"/>
       <c r="AC57" s="88"/>
     </row>
-    <row r="58" spans="1:29" ht="91.5">
+    <row r="58" spans="1:29" ht="29.5">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -10890,7 +11128,7 @@
       <c r="Y58"/>
       <c r="AC58" s="88"/>
     </row>
-    <row r="59" spans="1:29" ht="106.5">
+    <row r="59" spans="1:29" ht="29.5">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -10936,7 +11174,7 @@
       <c r="Y59"/>
       <c r="AC59" s="88"/>
     </row>
-    <row r="60" spans="1:29" ht="121.5">
+    <row r="60" spans="1:29" ht="44">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -10982,7 +11220,7 @@
       <c r="Y60"/>
       <c r="AC60" s="88"/>
     </row>
-    <row r="61" spans="1:29" ht="121.5">
+    <row r="61" spans="1:29" ht="44">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
@@ -11028,7 +11266,7 @@
       <c r="Y61"/>
       <c r="AC61" s="88"/>
     </row>
-    <row r="62" spans="1:29" ht="91.5">
+    <row r="62" spans="1:29" ht="29.5">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
@@ -11074,7 +11312,7 @@
       <c r="Y62"/>
       <c r="AC62" s="88"/>
     </row>
-    <row r="63" spans="1:29" ht="91.5">
+    <row r="63" spans="1:29" ht="29.5">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -11120,7 +11358,7 @@
       <c r="Y63"/>
       <c r="AC63" s="88"/>
     </row>
-    <row r="64" spans="1:29" ht="30.75">
+    <row r="64" spans="1:29" ht="16">
       <c r="A64"/>
       <c r="B64" t="s">
         <v>686</v>
@@ -11172,7 +11410,7 @@
       <c r="Y64"/>
       <c r="AC64" s="88"/>
     </row>
-    <row r="65" spans="1:29" ht="30.75">
+    <row r="65" spans="1:29" ht="29.5">
       <c r="A65"/>
       <c r="B65" t="s">
         <v>692</v>
@@ -11224,7 +11462,7 @@
       <c r="Y65"/>
       <c r="AC65" s="88"/>
     </row>
-    <row r="66" spans="1:29" ht="45.75">
+    <row r="66" spans="1:29" ht="44">
       <c r="B66"/>
       <c r="I66" s="82" t="s">
         <v>627</v>
@@ -11259,7 +11497,7 @@
       </c>
       <c r="AC66" s="88"/>
     </row>
-    <row r="67" spans="1:29" ht="45.75">
+    <row r="67" spans="1:29" ht="44">
       <c r="B67"/>
       <c r="I67" s="82" t="s">
         <v>627</v>
@@ -11294,7 +11532,7 @@
       </c>
       <c r="AC67" s="88"/>
     </row>
-    <row r="68" spans="1:29" ht="30.75">
+    <row r="68" spans="1:29" ht="16">
       <c r="B68"/>
       <c r="I68" s="82" t="s">
         <v>627</v>
@@ -11329,7 +11567,7 @@
       </c>
       <c r="AC68" s="88"/>
     </row>
-    <row r="69" spans="1:29" ht="45.75">
+    <row r="69" spans="1:29" ht="29.5">
       <c r="B69"/>
       <c r="I69" s="82" t="s">
         <v>627</v>
@@ -11364,7 +11602,7 @@
       </c>
       <c r="AC69" s="88"/>
     </row>
-    <row r="70" spans="1:29" ht="45.75">
+    <row r="70" spans="1:29" ht="29.5">
       <c r="B70"/>
       <c r="I70" s="82" t="s">
         <v>627</v>
@@ -11397,7 +11635,7 @@
       </c>
       <c r="AC70" s="88"/>
     </row>
-    <row r="71" spans="1:29" ht="45.75">
+    <row r="71" spans="1:29" ht="44">
       <c r="B71"/>
       <c r="I71" s="82" t="s">
         <v>627</v>
@@ -11430,7 +11668,7 @@
       </c>
       <c r="AC71" s="88"/>
     </row>
-    <row r="72" spans="1:29" ht="45.75">
+    <row r="72" spans="1:29" ht="16">
       <c r="B72"/>
       <c r="I72" s="82" t="s">
         <v>627</v>
@@ -11463,7 +11701,7 @@
       </c>
       <c r="AC72" s="88"/>
     </row>
-    <row r="73" spans="1:29" ht="45.75">
+    <row r="73" spans="1:29" ht="16">
       <c r="B73"/>
       <c r="I73" s="82" t="s">
         <v>627</v>
@@ -11496,7 +11734,7 @@
       </c>
       <c r="AC73" s="88"/>
     </row>
-    <row r="74" spans="1:29" ht="45.75">
+    <row r="74" spans="1:29" ht="29.5">
       <c r="B74"/>
       <c r="I74" s="82" t="s">
         <v>627</v>
@@ -11529,7 +11767,7 @@
       </c>
       <c r="AC74" s="88"/>
     </row>
-    <row r="75" spans="1:29" ht="60.75">
+    <row r="75" spans="1:29" ht="29.5">
       <c r="B75"/>
       <c r="I75" s="82" t="s">
         <v>627</v>
@@ -11562,7 +11800,7 @@
       </c>
       <c r="AC75" s="88"/>
     </row>
-    <row r="76" spans="1:29" ht="60.75">
+    <row r="76" spans="1:29" ht="29.5">
       <c r="B76"/>
       <c r="I76" s="82" t="s">
         <v>627</v>
@@ -11595,7 +11833,7 @@
       </c>
       <c r="AC76" s="88"/>
     </row>
-    <row r="77" spans="1:29" ht="30.75">
+    <row r="77" spans="1:29" ht="29.5">
       <c r="B77"/>
       <c r="I77" s="82" t="s">
         <v>627</v>
@@ -11628,7 +11866,7 @@
       </c>
       <c r="AC77" s="88"/>
     </row>
-    <row r="78" spans="1:29" ht="45.75">
+    <row r="78" spans="1:29" ht="29.5">
       <c r="B78"/>
       <c r="I78" s="82" t="s">
         <v>627</v>
@@ -11661,7 +11899,7 @@
       </c>
       <c r="AC78" s="88"/>
     </row>
-    <row r="79" spans="1:29" ht="45.75">
+    <row r="79" spans="1:29" ht="16">
       <c r="B79" s="108"/>
       <c r="I79" s="83" t="s">
         <v>708</v>
@@ -11696,7 +11934,7 @@
       </c>
       <c r="AC79" s="88"/>
     </row>
-    <row r="80" spans="1:29" ht="60.75">
+    <row r="80" spans="1:29" ht="29.5">
       <c r="B80" s="108"/>
       <c r="I80" s="83" t="s">
         <v>708</v>
@@ -11731,7 +11969,7 @@
       </c>
       <c r="AC80" s="88"/>
     </row>
-    <row r="81" spans="1:29" ht="30.75">
+    <row r="81" spans="1:29" ht="29.5">
       <c r="B81" s="108"/>
       <c r="I81" s="83" t="s">
         <v>708</v>
@@ -11764,7 +12002,7 @@
       </c>
       <c r="AC81" s="88"/>
     </row>
-    <row r="82" spans="1:29" ht="45.75">
+    <row r="82" spans="1:29" ht="16">
       <c r="B82" s="108"/>
       <c r="I82" s="83" t="s">
         <v>708</v>
@@ -11799,7 +12037,7 @@
       </c>
       <c r="AC82" s="88"/>
     </row>
-    <row r="83" spans="1:29" ht="76.5">
+    <row r="83" spans="1:29" ht="29.5">
       <c r="B83" s="108"/>
       <c r="I83" s="83" t="s">
         <v>708</v>
@@ -11834,7 +12072,7 @@
       </c>
       <c r="AC83" s="88"/>
     </row>
-    <row r="84" spans="1:29" ht="76.5">
+    <row r="84" spans="1:29" ht="29.5">
       <c r="B84" s="108"/>
       <c r="I84" s="83" t="s">
         <v>708</v>
@@ -11869,7 +12107,7 @@
       </c>
       <c r="AC84" s="88"/>
     </row>
-    <row r="85" spans="1:29" ht="30.75">
+    <row r="85" spans="1:29" ht="29.5">
       <c r="A85"/>
       <c r="B85" t="s">
         <v>724</v>
@@ -11921,7 +12159,7 @@
       <c r="Y85"/>
       <c r="AC85" s="88"/>
     </row>
-    <row r="86" spans="1:29" ht="30.75">
+    <row r="86" spans="1:29" ht="29.5">
       <c r="A86"/>
       <c r="B86" t="s">
         <v>728</v>
@@ -11973,7 +12211,7 @@
       <c r="Y86"/>
       <c r="AC86" s="88"/>
     </row>
-    <row r="87" spans="1:29" ht="45.75">
+    <row r="87" spans="1:29" ht="44">
       <c r="B87"/>
       <c r="I87" s="82" t="s">
         <v>627</v>
@@ -12008,7 +12246,7 @@
       </c>
       <c r="AC87" s="88"/>
     </row>
-    <row r="88" spans="1:29" ht="45.75">
+    <row r="88" spans="1:29" ht="44">
       <c r="B88"/>
       <c r="I88" s="82" t="s">
         <v>627</v>
@@ -12043,7 +12281,7 @@
       </c>
       <c r="AC88" s="88"/>
     </row>
-    <row r="89" spans="1:29" ht="30.75">
+    <row r="89" spans="1:29" ht="29.5">
       <c r="B89"/>
       <c r="I89" s="82" t="s">
         <v>627</v>
@@ -12078,7 +12316,7 @@
       </c>
       <c r="AC89" s="88"/>
     </row>
-    <row r="90" spans="1:29" ht="30.75">
+    <row r="90" spans="1:29" ht="29.5">
       <c r="B90"/>
       <c r="I90" s="82" t="s">
         <v>627</v>
@@ -12113,7 +12351,7 @@
       </c>
       <c r="AC90" s="88"/>
     </row>
-    <row r="91" spans="1:29" ht="30.75">
+    <row r="91" spans="1:29" ht="29.5">
       <c r="B91"/>
       <c r="I91" s="82" t="s">
         <v>627</v>
@@ -12146,7 +12384,7 @@
       </c>
       <c r="AC91" s="88"/>
     </row>
-    <row r="92" spans="1:29" ht="45.75">
+    <row r="92" spans="1:29" ht="44">
       <c r="B92"/>
       <c r="I92" s="82" t="s">
         <v>627</v>
@@ -12179,7 +12417,7 @@
       </c>
       <c r="AC92" s="88"/>
     </row>
-    <row r="93" spans="1:29" ht="30.75">
+    <row r="93" spans="1:29" ht="29.5">
       <c r="B93"/>
       <c r="I93" s="82" t="s">
         <v>627</v>
@@ -12212,7 +12450,7 @@
       </c>
       <c r="AC93" s="88"/>
     </row>
-    <row r="94" spans="1:29" ht="30.75">
+    <row r="94" spans="1:29" ht="29.5">
       <c r="B94"/>
       <c r="I94" s="82" t="s">
         <v>627</v>
@@ -12245,7 +12483,7 @@
       </c>
       <c r="AC94" s="88"/>
     </row>
-    <row r="95" spans="1:29" ht="30.75">
+    <row r="95" spans="1:29" ht="29.5">
       <c r="B95"/>
       <c r="I95" s="82" t="s">
         <v>627</v>
@@ -12278,7 +12516,7 @@
       </c>
       <c r="AC95" s="88"/>
     </row>
-    <row r="96" spans="1:29" ht="30.75">
+    <row r="96" spans="1:29" ht="44">
       <c r="B96"/>
       <c r="I96" s="82" t="s">
         <v>627</v>
@@ -12311,7 +12549,7 @@
       </c>
       <c r="AC96" s="88"/>
     </row>
-    <row r="97" spans="1:29" ht="30.75">
+    <row r="97" spans="1:29" ht="44">
       <c r="B97"/>
       <c r="I97" s="82" t="s">
         <v>627</v>
@@ -12344,7 +12582,7 @@
       </c>
       <c r="AC97" s="88"/>
     </row>
-    <row r="98" spans="1:29" ht="30.75">
+    <row r="98" spans="1:29" ht="29.5">
       <c r="B98"/>
       <c r="I98" s="82" t="s">
         <v>627</v>
@@ -12377,7 +12615,7 @@
       </c>
       <c r="AC98" s="88"/>
     </row>
-    <row r="99" spans="1:29" ht="30.75">
+    <row r="99" spans="1:29" ht="29.5">
       <c r="B99"/>
       <c r="I99" s="82" t="s">
         <v>627</v>
@@ -12410,7 +12648,7 @@
       </c>
       <c r="AC99" s="88"/>
     </row>
-    <row r="100" spans="1:29" ht="30.75">
+    <row r="100" spans="1:29" ht="29.5">
       <c r="B100" s="108"/>
       <c r="I100" s="83" t="s">
         <v>708</v>
@@ -12445,7 +12683,7 @@
       </c>
       <c r="AC100" s="88"/>
     </row>
-    <row r="101" spans="1:29" ht="30.75">
+    <row r="101" spans="1:29" ht="29.5">
       <c r="B101" s="108"/>
       <c r="I101" s="83" t="s">
         <v>708</v>
@@ -12480,7 +12718,7 @@
       </c>
       <c r="AC101" s="88"/>
     </row>
-    <row r="102" spans="1:29" ht="45.75">
+    <row r="102" spans="1:29" ht="44">
       <c r="B102" s="108"/>
       <c r="I102" s="83" t="s">
         <v>708</v>
@@ -12510,7 +12748,7 @@
       </c>
       <c r="AC102" s="88"/>
     </row>
-    <row r="103" spans="1:29" ht="30.75">
+    <row r="103" spans="1:29" ht="29.5">
       <c r="B103" s="108"/>
       <c r="I103" s="83" t="s">
         <v>708</v>
@@ -12545,7 +12783,7 @@
       </c>
       <c r="AC103" s="88"/>
     </row>
-    <row r="104" spans="1:29" ht="30.75">
+    <row r="104" spans="1:29" ht="44">
       <c r="B104" s="108"/>
       <c r="I104" s="83" t="s">
         <v>708</v>
@@ -12580,7 +12818,7 @@
       </c>
       <c r="AC104" s="88"/>
     </row>
-    <row r="105" spans="1:29" ht="45.75">
+    <row r="105" spans="1:29" ht="44">
       <c r="B105" s="108"/>
       <c r="I105" s="83" t="s">
         <v>708</v>
@@ -12615,7 +12853,7 @@
       </c>
       <c r="AC105" s="88"/>
     </row>
-    <row r="106" spans="1:29" ht="60.75">
+    <row r="106" spans="1:29" ht="16">
       <c r="A106"/>
       <c r="B106" t="s">
         <v>750</v>
@@ -12667,7 +12905,7 @@
       <c r="Y106"/>
       <c r="AC106" s="88"/>
     </row>
-    <row r="107" spans="1:29" ht="30.75">
+    <row r="107" spans="1:29" ht="29.5">
       <c r="A107"/>
       <c r="B107" t="s">
         <v>756</v>
@@ -12719,7 +12957,7 @@
       <c r="Y107"/>
       <c r="AC107" s="88"/>
     </row>
-    <row r="108" spans="1:29" ht="45.75">
+    <row r="108" spans="1:29" ht="44">
       <c r="A108"/>
       <c r="B108" t="s">
         <v>762</v>
@@ -12771,7 +13009,7 @@
       <c r="Y108"/>
       <c r="AC108" s="88"/>
     </row>
-    <row r="109" spans="1:29" ht="45.75">
+    <row r="109" spans="1:29" ht="44">
       <c r="A109"/>
       <c r="B109" t="s">
         <v>769</v>
@@ -12823,7 +13061,7 @@
       <c r="Y109"/>
       <c r="AC109" s="88"/>
     </row>
-    <row r="110" spans="1:29" ht="45.75">
+    <row r="110" spans="1:29" ht="44">
       <c r="A110"/>
       <c r="B110" t="s">
         <v>775</v>
@@ -12875,7 +13113,7 @@
       <c r="Y110"/>
       <c r="AC110" s="88"/>
     </row>
-    <row r="111" spans="1:29" ht="60.75">
+    <row r="111" spans="1:29" ht="29.5">
       <c r="A111"/>
       <c r="B111" t="s">
         <v>780</v>
@@ -12927,7 +13165,7 @@
       <c r="Y111"/>
       <c r="AC111" s="88"/>
     </row>
-    <row r="112" spans="1:29" ht="76.5">
+    <row r="112" spans="1:29" ht="29.5">
       <c r="A112"/>
       <c r="B112" t="s">
         <v>783</v>
@@ -12979,7 +13217,7 @@
       <c r="Y112"/>
       <c r="AC112" s="88"/>
     </row>
-    <row r="113" spans="1:29" ht="45.75">
+    <row r="113" spans="1:29" ht="44">
       <c r="A113"/>
       <c r="B113" t="s">
         <v>786</v>
@@ -13031,7 +13269,7 @@
       <c r="Y113"/>
       <c r="AC113" s="88"/>
     </row>
-    <row r="114" spans="1:29" ht="121.5">
+    <row r="114" spans="1:29" ht="44">
       <c r="A114"/>
       <c r="B114" t="s">
         <v>789</v>
@@ -13083,7 +13321,7 @@
       <c r="Y114"/>
       <c r="AC114" s="88"/>
     </row>
-    <row r="115" spans="1:29" ht="137.25">
+    <row r="115" spans="1:29" ht="44">
       <c r="A115"/>
       <c r="B115" t="s">
         <v>792</v>
@@ -13135,7 +13373,7 @@
       <c r="Y115"/>
       <c r="AC115" s="88"/>
     </row>
-    <row r="116" spans="1:29" ht="15.75">
+    <row r="116" spans="1:29" ht="16">
       <c r="A116"/>
       <c r="B116"/>
       <c r="C116"/>
@@ -13162,7 +13400,7 @@
       <c r="Y116"/>
       <c r="AC116" s="88"/>
     </row>
-    <row r="117" spans="1:29" ht="15.75">
+    <row r="117" spans="1:29" ht="16">
       <c r="A117"/>
       <c r="B117"/>
       <c r="C117"/>
@@ -13189,7 +13427,7 @@
       <c r="Y117"/>
       <c r="AC117" s="88"/>
     </row>
-    <row r="118" spans="1:29" ht="15.75">
+    <row r="118" spans="1:29" ht="16">
       <c r="A118"/>
       <c r="B118"/>
       <c r="C118"/>
@@ -13216,7 +13454,7 @@
       <c r="Y118"/>
       <c r="AC118" s="88"/>
     </row>
-    <row r="119" spans="1:29" ht="15.75">
+    <row r="119" spans="1:29" ht="16">
       <c r="A119"/>
       <c r="B119"/>
       <c r="C119"/>
@@ -13243,7 +13481,7 @@
       <c r="Y119"/>
       <c r="AC119" s="88"/>
     </row>
-    <row r="120" spans="1:29" ht="15.75">
+    <row r="120" spans="1:29" ht="16">
       <c r="A120"/>
       <c r="B120"/>
       <c r="C120"/>
@@ -13270,7 +13508,7 @@
       <c r="Y120"/>
       <c r="AC120" s="88"/>
     </row>
-    <row r="121" spans="1:29" ht="15.75">
+    <row r="121" spans="1:29" ht="16">
       <c r="A121"/>
       <c r="B121"/>
       <c r="C121"/>
@@ -13297,7 +13535,7 @@
       <c r="Y121"/>
       <c r="AC121" s="88"/>
     </row>
-    <row r="122" spans="1:29" ht="15.75">
+    <row r="122" spans="1:29" ht="16">
       <c r="A122"/>
       <c r="B122"/>
       <c r="C122"/>
@@ -13324,7 +13562,7 @@
       <c r="Y122"/>
       <c r="AC122" s="88"/>
     </row>
-    <row r="123" spans="1:29" ht="15.75">
+    <row r="123" spans="1:29" ht="16">
       <c r="A123"/>
       <c r="B123"/>
       <c r="C123"/>
@@ -13350,7 +13588,7 @@
       <c r="Y123"/>
       <c r="AC123" s="88"/>
     </row>
-    <row r="124" spans="1:29" ht="15.75">
+    <row r="124" spans="1:29" ht="16">
       <c r="A124"/>
       <c r="B124"/>
       <c r="C124"/>
@@ -13376,7 +13614,7 @@
       <c r="Y124"/>
       <c r="AC124" s="88"/>
     </row>
-    <row r="125" spans="1:29" ht="15.75">
+    <row r="125" spans="1:29" ht="16">
       <c r="A125"/>
       <c r="B125"/>
       <c r="C125"/>
@@ -13402,7 +13640,7 @@
       <c r="Y125"/>
       <c r="AC125" s="88"/>
     </row>
-    <row r="126" spans="1:29" ht="15.75">
+    <row r="126" spans="1:29" ht="16">
       <c r="A126"/>
       <c r="B126"/>
       <c r="C126"/>
@@ -13428,7 +13666,7 @@
       <c r="Y126"/>
       <c r="AC126" s="88"/>
     </row>
-    <row r="127" spans="1:29" ht="15.75">
+    <row r="127" spans="1:29" ht="16">
       <c r="A127"/>
       <c r="B127"/>
       <c r="C127"/>
@@ -13454,7 +13692,7 @@
       <c r="Y127"/>
       <c r="AC127" s="88"/>
     </row>
-    <row r="128" spans="1:29" ht="15.75">
+    <row r="128" spans="1:29" ht="16">
       <c r="A128"/>
       <c r="B128"/>
       <c r="C128"/>
@@ -13480,7 +13718,7 @@
       <c r="Y128"/>
       <c r="AC128" s="88"/>
     </row>
-    <row r="129" spans="1:29" ht="15.75">
+    <row r="129" spans="1:29" ht="16">
       <c r="A129"/>
       <c r="B129"/>
       <c r="C129"/>
@@ -13506,7 +13744,7 @@
       <c r="Y129"/>
       <c r="AC129" s="88"/>
     </row>
-    <row r="130" spans="1:29" ht="15.75">
+    <row r="130" spans="1:29" ht="16">
       <c r="A130"/>
       <c r="B130"/>
       <c r="C130"/>
@@ -13532,7 +13770,7 @@
       <c r="Y130"/>
       <c r="AC130" s="88"/>
     </row>
-    <row r="131" spans="1:29" ht="15.75">
+    <row r="131" spans="1:29" ht="16">
       <c r="A131"/>
       <c r="B131"/>
       <c r="C131"/>
@@ -13559,7 +13797,7 @@
       <c r="Y131"/>
       <c r="AC131" s="88"/>
     </row>
-    <row r="132" spans="1:29" ht="15.75">
+    <row r="132" spans="1:29" ht="16">
       <c r="A132"/>
       <c r="B132"/>
       <c r="C132"/>
@@ -13585,7 +13823,7 @@
       <c r="Y132"/>
       <c r="AC132" s="88"/>
     </row>
-    <row r="133" spans="1:29" ht="15.75">
+    <row r="133" spans="1:29" ht="16">
       <c r="A133"/>
       <c r="B133"/>
       <c r="C133"/>
@@ -13612,7 +13850,7 @@
       <c r="Y133"/>
       <c r="AC133" s="88"/>
     </row>
-    <row r="134" spans="1:29" ht="15.75">
+    <row r="134" spans="1:29" ht="16">
       <c r="A134"/>
       <c r="B134"/>
       <c r="C134"/>
@@ -13639,7 +13877,7 @@
       <c r="Y134"/>
       <c r="AC134" s="88"/>
     </row>
-    <row r="135" spans="1:29" ht="15.75">
+    <row r="135" spans="1:29" ht="16">
       <c r="A135"/>
       <c r="B135"/>
       <c r="C135"/>
@@ -13666,7 +13904,7 @@
       <c r="Y135"/>
       <c r="AC135" s="88"/>
     </row>
-    <row r="136" spans="1:29" ht="15.75">
+    <row r="136" spans="1:29" ht="16">
       <c r="A136"/>
       <c r="B136"/>
       <c r="C136"/>
@@ -13692,7 +13930,7 @@
       <c r="Y136"/>
       <c r="AC136" s="88"/>
     </row>
-    <row r="137" spans="1:29" ht="15.75">
+    <row r="137" spans="1:29" ht="16">
       <c r="A137"/>
       <c r="B137"/>
       <c r="C137"/>
@@ -13719,7 +13957,7 @@
       <c r="Y137"/>
       <c r="AC137" s="88"/>
     </row>
-    <row r="138" spans="1:29" ht="15.75">
+    <row r="138" spans="1:29" ht="16">
       <c r="A138"/>
       <c r="B138"/>
       <c r="C138"/>
@@ -13746,7 +13984,7 @@
       <c r="Y138"/>
       <c r="AC138" s="88"/>
     </row>
-    <row r="139" spans="1:29" ht="15.75">
+    <row r="139" spans="1:29" ht="16">
       <c r="A139"/>
       <c r="B139"/>
       <c r="C139"/>
@@ -13773,7 +14011,7 @@
       <c r="Y139"/>
       <c r="AC139" s="88"/>
     </row>
-    <row r="140" spans="1:29" ht="15.75">
+    <row r="140" spans="1:29" ht="16">
       <c r="A140"/>
       <c r="B140"/>
       <c r="C140"/>
@@ -13800,7 +14038,7 @@
       <c r="Y140"/>
       <c r="AC140" s="88"/>
     </row>
-    <row r="141" spans="1:29" ht="15.75">
+    <row r="141" spans="1:29" ht="16">
       <c r="A141"/>
       <c r="B141"/>
       <c r="C141"/>
@@ -13827,7 +14065,7 @@
       <c r="Y141"/>
       <c r="AC141" s="88"/>
     </row>
-    <row r="142" spans="1:29" ht="15.75">
+    <row r="142" spans="1:29" ht="16">
       <c r="A142"/>
       <c r="B142"/>
       <c r="C142"/>
@@ -13881,7 +14119,7 @@
       <c r="Y143"/>
       <c r="AC143" s="83"/>
     </row>
-    <row r="144" spans="1:29" ht="15.75">
+    <row r="144" spans="1:29" ht="16">
       <c r="A144"/>
       <c r="B144"/>
       <c r="C144"/>
@@ -13908,7 +14146,7 @@
       <c r="Y144"/>
       <c r="AC144" s="88"/>
     </row>
-    <row r="145" spans="1:29" ht="15.75">
+    <row r="145" spans="1:29" ht="16">
       <c r="A145"/>
       <c r="B145"/>
       <c r="C145"/>
@@ -13935,7 +14173,7 @@
       <c r="Y145"/>
       <c r="AC145" s="94"/>
     </row>
-    <row r="146" spans="1:29" ht="15.75">
+    <row r="146" spans="1:29" ht="16">
       <c r="A146"/>
       <c r="B146"/>
       <c r="C146"/>
@@ -13962,7 +14200,7 @@
       <c r="Y146"/>
       <c r="AC146" s="88"/>
     </row>
-    <row r="147" spans="1:29" ht="15.75">
+    <row r="147" spans="1:29" ht="16">
       <c r="A147"/>
       <c r="B147"/>
       <c r="C147"/>
@@ -13989,7 +14227,7 @@
       <c r="Y147"/>
       <c r="AC147" s="88"/>
     </row>
-    <row r="148" spans="1:29" ht="15.75">
+    <row r="148" spans="1:29" ht="16">
       <c r="A148"/>
       <c r="B148"/>
       <c r="C148"/>
@@ -14016,7 +14254,7 @@
       <c r="Y148"/>
       <c r="AC148" s="88"/>
     </row>
-    <row r="149" spans="1:29" ht="15.75">
+    <row r="149" spans="1:29" ht="16">
       <c r="A149"/>
       <c r="B149"/>
       <c r="C149"/>
@@ -14043,7 +14281,7 @@
       <c r="Y149"/>
       <c r="AC149" s="88"/>
     </row>
-    <row r="150" spans="1:29" ht="15.75">
+    <row r="150" spans="1:29" ht="16">
       <c r="A150"/>
       <c r="B150"/>
       <c r="C150"/>
@@ -14070,7 +14308,7 @@
       <c r="Y150"/>
       <c r="AC150" s="88"/>
     </row>
-    <row r="151" spans="1:29" ht="15.75">
+    <row r="151" spans="1:29" ht="16">
       <c r="A151"/>
       <c r="B151"/>
       <c r="C151"/>
@@ -14096,7 +14334,7 @@
       <c r="Y151"/>
       <c r="AC151" s="88"/>
     </row>
-    <row r="152" spans="1:29" ht="15.75">
+    <row r="152" spans="1:29" ht="16">
       <c r="A152"/>
       <c r="B152"/>
       <c r="C152"/>
@@ -14123,7 +14361,7 @@
       <c r="Y152"/>
       <c r="AC152" s="88"/>
     </row>
-    <row r="153" spans="1:29" ht="15.75">
+    <row r="153" spans="1:29" ht="16">
       <c r="A153"/>
       <c r="B153"/>
       <c r="C153"/>
@@ -14150,7 +14388,7 @@
       <c r="Y153"/>
       <c r="AC153" s="88"/>
     </row>
-    <row r="154" spans="1:29" ht="15.75">
+    <row r="154" spans="1:29" ht="16">
       <c r="A154"/>
       <c r="B154"/>
       <c r="C154"/>
@@ -14177,7 +14415,7 @@
       <c r="Y154"/>
       <c r="AC154" s="88"/>
     </row>
-    <row r="155" spans="1:29" ht="15.75">
+    <row r="155" spans="1:29" ht="16">
       <c r="A155"/>
       <c r="B155"/>
       <c r="C155"/>
@@ -14204,7 +14442,7 @@
       <c r="Y155"/>
       <c r="AC155" s="88"/>
     </row>
-    <row r="156" spans="1:29" ht="15.75">
+    <row r="156" spans="1:29" ht="16">
       <c r="A156"/>
       <c r="B156"/>
       <c r="C156"/>
@@ -14231,7 +14469,7 @@
       <c r="Y156"/>
       <c r="AC156" s="88"/>
     </row>
-    <row r="157" spans="1:29" ht="15.75">
+    <row r="157" spans="1:29" ht="16">
       <c r="A157"/>
       <c r="B157"/>
       <c r="C157"/>
@@ -14258,7 +14496,7 @@
       <c r="Y157"/>
       <c r="AC157" s="88"/>
     </row>
-    <row r="158" spans="1:29" ht="15.75">
+    <row r="158" spans="1:29" ht="16">
       <c r="A158"/>
       <c r="B158"/>
       <c r="C158"/>
@@ -14285,7 +14523,7 @@
       <c r="Y158"/>
       <c r="AC158" s="88"/>
     </row>
-    <row r="159" spans="1:29" ht="15.75">
+    <row r="159" spans="1:29" ht="16">
       <c r="A159"/>
       <c r="B159"/>
       <c r="C159"/>
@@ -14312,7 +14550,7 @@
       <c r="Y159"/>
       <c r="AC159" s="88"/>
     </row>
-    <row r="160" spans="1:29" ht="15.75">
+    <row r="160" spans="1:29" ht="16">
       <c r="A160"/>
       <c r="B160"/>
       <c r="C160"/>
@@ -14339,7 +14577,7 @@
       <c r="Y160"/>
       <c r="AC160" s="88"/>
     </row>
-    <row r="161" spans="1:29" ht="15.75">
+    <row r="161" spans="1:29" ht="16">
       <c r="A161"/>
       <c r="B161"/>
       <c r="C161"/>
@@ -14366,7 +14604,7 @@
       <c r="Y161"/>
       <c r="AC161" s="88"/>
     </row>
-    <row r="162" spans="1:29" ht="15.75">
+    <row r="162" spans="1:29" ht="16">
       <c r="A162"/>
       <c r="B162"/>
       <c r="C162"/>
@@ -14393,7 +14631,7 @@
       <c r="Y162"/>
       <c r="AC162" s="88"/>
     </row>
-    <row r="163" spans="1:29" ht="15.75">
+    <row r="163" spans="1:29" ht="16">
       <c r="A163"/>
       <c r="B163"/>
       <c r="C163"/>
@@ -14420,7 +14658,7 @@
       <c r="Y163"/>
       <c r="AC163" s="88"/>
     </row>
-    <row r="164" spans="1:29" ht="15.75">
+    <row r="164" spans="1:29" ht="16">
       <c r="A164"/>
       <c r="B164"/>
       <c r="C164"/>
@@ -14447,7 +14685,7 @@
       <c r="Y164"/>
       <c r="AC164" s="88"/>
     </row>
-    <row r="165" spans="1:29" ht="15.75">
+    <row r="165" spans="1:29" ht="16">
       <c r="A165"/>
       <c r="B165"/>
       <c r="C165"/>
@@ -14474,7 +14712,7 @@
       <c r="Y165"/>
       <c r="AC165" s="88"/>
     </row>
-    <row r="166" spans="1:29" ht="15.75">
+    <row r="166" spans="1:29" ht="16">
       <c r="A166"/>
       <c r="B166"/>
       <c r="C166"/>
@@ -14500,7 +14738,7 @@
       <c r="Y166"/>
       <c r="AC166" s="88"/>
     </row>
-    <row r="167" spans="1:29" ht="15.75">
+    <row r="167" spans="1:29" ht="16">
       <c r="A167"/>
       <c r="B167"/>
       <c r="C167"/>
@@ -14526,7 +14764,7 @@
       <c r="Y167"/>
       <c r="AC167" s="88"/>
     </row>
-    <row r="168" spans="1:29" ht="15.75">
+    <row r="168" spans="1:29" ht="16">
       <c r="A168"/>
       <c r="B168"/>
       <c r="C168"/>
@@ -14552,7 +14790,7 @@
       <c r="Y168"/>
       <c r="AC168" s="88"/>
     </row>
-    <row r="169" spans="1:29" ht="15.75">
+    <row r="169" spans="1:29" ht="16">
       <c r="A169"/>
       <c r="B169"/>
       <c r="C169"/>
@@ -14578,7 +14816,7 @@
       <c r="Y169"/>
       <c r="AC169" s="88"/>
     </row>
-    <row r="170" spans="1:29" ht="15.75">
+    <row r="170" spans="1:29" ht="16">
       <c r="A170"/>
       <c r="B170"/>
       <c r="C170"/>
@@ -14604,7 +14842,7 @@
       <c r="Y170"/>
       <c r="AC170" s="88"/>
     </row>
-    <row r="171" spans="1:29" ht="15.75">
+    <row r="171" spans="1:29" ht="16">
       <c r="A171"/>
       <c r="B171"/>
       <c r="C171"/>
@@ -14630,7 +14868,7 @@
       <c r="Y171"/>
       <c r="AC171" s="88"/>
     </row>
-    <row r="172" spans="1:29" ht="15.75">
+    <row r="172" spans="1:29" ht="16">
       <c r="A172"/>
       <c r="B172"/>
       <c r="C172"/>
@@ -14656,7 +14894,7 @@
       <c r="Y172"/>
       <c r="AC172" s="88"/>
     </row>
-    <row r="173" spans="1:29" ht="15.75">
+    <row r="173" spans="1:29" ht="16">
       <c r="A173"/>
       <c r="B173"/>
       <c r="C173"/>
@@ -14682,7 +14920,7 @@
       <c r="Y173"/>
       <c r="AC173" s="88"/>
     </row>
-    <row r="174" spans="1:29" ht="15.75">
+    <row r="174" spans="1:29" ht="16">
       <c r="A174"/>
       <c r="B174"/>
       <c r="C174"/>
@@ -14708,7 +14946,7 @@
       <c r="Y174"/>
       <c r="AC174" s="88"/>
     </row>
-    <row r="175" spans="1:29" ht="15.75">
+    <row r="175" spans="1:29" ht="16">
       <c r="A175"/>
       <c r="B175"/>
       <c r="C175"/>
@@ -14734,7 +14972,7 @@
       <c r="Y175"/>
       <c r="AC175" s="88"/>
     </row>
-    <row r="176" spans="1:29" ht="15.75">
+    <row r="176" spans="1:29" ht="16">
       <c r="A176"/>
       <c r="B176"/>
       <c r="C176"/>
@@ -14760,7 +14998,7 @@
       <c r="Y176"/>
       <c r="AC176" s="88"/>
     </row>
-    <row r="177" spans="1:29" ht="15.75">
+    <row r="177" spans="1:29" ht="16">
       <c r="A177"/>
       <c r="B177"/>
       <c r="C177"/>
@@ -14786,7 +15024,7 @@
       <c r="Y177"/>
       <c r="AC177" s="88"/>
     </row>
-    <row r="178" spans="1:29" ht="15.75">
+    <row r="178" spans="1:29" ht="16">
       <c r="A178"/>
       <c r="B178"/>
       <c r="C178"/>
@@ -14812,7 +15050,7 @@
       <c r="Y178"/>
       <c r="AC178" s="88"/>
     </row>
-    <row r="179" spans="1:29" ht="15.75">
+    <row r="179" spans="1:29" ht="16">
       <c r="A179"/>
       <c r="B179"/>
       <c r="C179"/>
@@ -14838,7 +15076,7 @@
       <c r="Y179"/>
       <c r="AC179" s="88"/>
     </row>
-    <row r="180" spans="1:29" ht="15.75">
+    <row r="180" spans="1:29" ht="16">
       <c r="A180"/>
       <c r="B180"/>
       <c r="C180"/>
@@ -14864,7 +15102,7 @@
       <c r="Y180"/>
       <c r="AC180" s="88"/>
     </row>
-    <row r="181" spans="1:29" ht="15.75">
+    <row r="181" spans="1:29" ht="16">
       <c r="A181"/>
       <c r="B181"/>
       <c r="C181"/>
@@ -14890,7 +15128,7 @@
       <c r="Y181"/>
       <c r="AC181" s="88"/>
     </row>
-    <row r="182" spans="1:29" ht="15.75">
+    <row r="182" spans="1:29" ht="16">
       <c r="A182"/>
       <c r="B182"/>
       <c r="C182"/>
@@ -14916,7 +15154,7 @@
       <c r="Y182"/>
       <c r="AC182" s="88"/>
     </row>
-    <row r="183" spans="1:29" ht="15.75">
+    <row r="183" spans="1:29" ht="16">
       <c r="A183"/>
       <c r="B183"/>
       <c r="C183"/>
@@ -14942,7 +15180,7 @@
       <c r="Y183"/>
       <c r="AC183" s="88"/>
     </row>
-    <row r="184" spans="1:29" ht="15.75">
+    <row r="184" spans="1:29" ht="16">
       <c r="A184"/>
       <c r="B184"/>
       <c r="C184"/>
@@ -14968,7 +15206,7 @@
       <c r="Y184"/>
       <c r="AC184" s="88"/>
     </row>
-    <row r="185" spans="1:29" ht="15.75">
+    <row r="185" spans="1:29" ht="16">
       <c r="A185"/>
       <c r="B185"/>
       <c r="C185"/>
@@ -14994,7 +15232,7 @@
       <c r="Y185"/>
       <c r="AC185" s="88"/>
     </row>
-    <row r="186" spans="1:29" ht="15.75">
+    <row r="186" spans="1:29" ht="16">
       <c r="A186"/>
       <c r="B186"/>
       <c r="C186"/>
@@ -15020,7 +15258,7 @@
       <c r="Y186"/>
       <c r="AC186" s="88"/>
     </row>
-    <row r="187" spans="1:29" ht="15.75">
+    <row r="187" spans="1:29" ht="16">
       <c r="A187"/>
       <c r="B187"/>
       <c r="C187"/>
@@ -15046,7 +15284,7 @@
       <c r="Y187"/>
       <c r="AC187" s="88"/>
     </row>
-    <row r="188" spans="1:29" ht="15.75">
+    <row r="188" spans="1:29" ht="16">
       <c r="A188"/>
       <c r="B188"/>
       <c r="C188"/>
@@ -15072,7 +15310,7 @@
       <c r="Y188"/>
       <c r="AC188" s="88"/>
     </row>
-    <row r="189" spans="1:29" ht="15.75">
+    <row r="189" spans="1:29" ht="16">
       <c r="A189"/>
       <c r="B189"/>
       <c r="C189"/>
@@ -15098,7 +15336,7 @@
       <c r="Y189"/>
       <c r="AC189" s="88"/>
     </row>
-    <row r="190" spans="1:29" ht="15.75">
+    <row r="190" spans="1:29" ht="16">
       <c r="A190"/>
       <c r="B190"/>
       <c r="C190"/>
@@ -15124,7 +15362,7 @@
       <c r="Y190"/>
       <c r="AC190" s="88"/>
     </row>
-    <row r="191" spans="1:29" ht="15.75">
+    <row r="191" spans="1:29" ht="16">
       <c r="A191"/>
       <c r="B191"/>
       <c r="C191"/>
@@ -15150,7 +15388,7 @@
       <c r="Y191"/>
       <c r="AC191" s="88"/>
     </row>
-    <row r="192" spans="1:29" ht="15.75">
+    <row r="192" spans="1:29" ht="16">
       <c r="A192"/>
       <c r="B192"/>
       <c r="C192"/>
@@ -15176,7 +15414,7 @@
       <c r="Y192"/>
       <c r="AC192" s="88"/>
     </row>
-    <row r="193" spans="1:29" ht="15.75">
+    <row r="193" spans="1:29" ht="16">
       <c r="A193"/>
       <c r="B193"/>
       <c r="C193"/>
@@ -15202,7 +15440,7 @@
       <c r="Y193"/>
       <c r="AC193" s="88"/>
     </row>
-    <row r="194" spans="1:29" ht="15.75">
+    <row r="194" spans="1:29" ht="16">
       <c r="A194"/>
       <c r="B194"/>
       <c r="C194"/>
@@ -15228,7 +15466,7 @@
       <c r="Y194"/>
       <c r="AC194" s="88"/>
     </row>
-    <row r="195" spans="1:29" ht="15.75">
+    <row r="195" spans="1:29" ht="16">
       <c r="A195"/>
       <c r="B195"/>
       <c r="C195"/>
@@ -15254,7 +15492,7 @@
       <c r="Y195"/>
       <c r="AC195" s="88"/>
     </row>
-    <row r="196" spans="1:29" ht="15.75">
+    <row r="196" spans="1:29" ht="16">
       <c r="A196"/>
       <c r="B196"/>
       <c r="C196"/>
@@ -15280,7 +15518,7 @@
       <c r="Y196"/>
       <c r="AC196" s="88"/>
     </row>
-    <row r="197" spans="1:29" ht="15.75">
+    <row r="197" spans="1:29" ht="16">
       <c r="A197"/>
       <c r="B197"/>
       <c r="C197"/>
@@ -15306,7 +15544,7 @@
       <c r="Y197"/>
       <c r="AC197" s="88"/>
     </row>
-    <row r="198" spans="1:29" ht="15.75">
+    <row r="198" spans="1:29" ht="16">
       <c r="A198"/>
       <c r="B198"/>
       <c r="C198"/>
@@ -15332,7 +15570,7 @@
       <c r="Y198"/>
       <c r="AC198" s="88"/>
     </row>
-    <row r="199" spans="1:29" ht="15.75">
+    <row r="199" spans="1:29" ht="16">
       <c r="A199"/>
       <c r="B199"/>
       <c r="C199"/>
@@ -15358,7 +15596,7 @@
       <c r="Y199"/>
       <c r="AC199" s="88"/>
     </row>
-    <row r="200" spans="1:29" ht="15.75">
+    <row r="200" spans="1:29" ht="16">
       <c r="A200"/>
       <c r="B200"/>
       <c r="C200"/>
@@ -15384,7 +15622,7 @@
       <c r="Y200"/>
       <c r="AC200" s="88"/>
     </row>
-    <row r="201" spans="1:29" ht="15.75">
+    <row r="201" spans="1:29" ht="16">
       <c r="A201"/>
       <c r="B201"/>
       <c r="C201"/>
@@ -15410,7 +15648,7 @@
       <c r="Y201"/>
       <c r="AC201" s="88"/>
     </row>
-    <row r="202" spans="1:29" ht="15.75">
+    <row r="202" spans="1:29" ht="16">
       <c r="A202"/>
       <c r="B202"/>
       <c r="C202"/>
@@ -15436,7 +15674,7 @@
       <c r="Y202"/>
       <c r="AC202" s="88"/>
     </row>
-    <row r="203" spans="1:29" ht="15.75">
+    <row r="203" spans="1:29" ht="16">
       <c r="A203"/>
       <c r="B203"/>
       <c r="C203"/>
@@ -15462,7 +15700,7 @@
       <c r="Y203"/>
       <c r="AC203" s="88"/>
     </row>
-    <row r="204" spans="1:29" ht="15.75">
+    <row r="204" spans="1:29" ht="16">
       <c r="A204"/>
       <c r="B204"/>
       <c r="C204"/>
@@ -15488,7 +15726,7 @@
       <c r="Y204"/>
       <c r="AC204" s="94"/>
     </row>
-    <row r="205" spans="1:29" ht="15.75">
+    <row r="205" spans="1:29" ht="16">
       <c r="A205"/>
       <c r="B205"/>
       <c r="C205"/>
@@ -15514,7 +15752,7 @@
       <c r="Y205"/>
       <c r="AC205" s="88"/>
     </row>
-    <row r="206" spans="1:29" ht="15.75">
+    <row r="206" spans="1:29" ht="16">
       <c r="A206"/>
       <c r="B206"/>
       <c r="C206"/>
@@ -15540,7 +15778,7 @@
       <c r="Y206"/>
       <c r="AC206" s="94"/>
     </row>
-    <row r="207" spans="1:29" ht="15.75">
+    <row r="207" spans="1:29" ht="16">
       <c r="A207"/>
       <c r="B207"/>
       <c r="C207"/>
@@ -15566,7 +15804,7 @@
       <c r="Y207"/>
       <c r="AC207" s="88"/>
     </row>
-    <row r="208" spans="1:29" ht="15.75">
+    <row r="208" spans="1:29" ht="16">
       <c r="A208"/>
       <c r="B208"/>
       <c r="C208"/>
@@ -15592,7 +15830,7 @@
       <c r="Y208"/>
       <c r="AC208" s="88"/>
     </row>
-    <row r="209" spans="1:29" ht="15.75">
+    <row r="209" spans="1:29" ht="16">
       <c r="A209"/>
       <c r="B209"/>
       <c r="C209"/>
@@ -15618,7 +15856,7 @@
       <c r="Y209"/>
       <c r="AC209" s="88"/>
     </row>
-    <row r="210" spans="1:29" ht="15.75">
+    <row r="210" spans="1:29" ht="16">
       <c r="A210"/>
       <c r="B210"/>
       <c r="C210"/>
@@ -15644,7 +15882,7 @@
       <c r="Y210"/>
       <c r="AC210" s="88"/>
     </row>
-    <row r="211" spans="1:29" ht="15.75">
+    <row r="211" spans="1:29" ht="16">
       <c r="A211"/>
       <c r="B211"/>
       <c r="C211"/>
@@ -15670,7 +15908,7 @@
       <c r="Y211"/>
       <c r="AC211" s="88"/>
     </row>
-    <row r="212" spans="1:29" ht="15.75">
+    <row r="212" spans="1:29" ht="16">
       <c r="A212"/>
       <c r="B212"/>
       <c r="C212"/>
@@ -15696,7 +15934,7 @@
       <c r="Y212"/>
       <c r="AC212" s="88"/>
     </row>
-    <row r="213" spans="1:29" ht="15.75">
+    <row r="213" spans="1:29" ht="16">
       <c r="A213"/>
       <c r="B213"/>
       <c r="C213"/>
@@ -15722,7 +15960,7 @@
       <c r="Y213"/>
       <c r="AC213" s="88"/>
     </row>
-    <row r="214" spans="1:29" ht="15.75">
+    <row r="214" spans="1:29" ht="16">
       <c r="A214"/>
       <c r="B214"/>
       <c r="C214"/>
@@ -15748,7 +15986,7 @@
       <c r="Y214"/>
       <c r="AC214" s="88"/>
     </row>
-    <row r="215" spans="1:29" ht="15.75">
+    <row r="215" spans="1:29" ht="16">
       <c r="A215"/>
       <c r="B215"/>
       <c r="C215"/>
@@ -15774,7 +16012,7 @@
       <c r="Y215"/>
       <c r="AC215" s="88"/>
     </row>
-    <row r="216" spans="1:29" ht="15.75">
+    <row r="216" spans="1:29" ht="16">
       <c r="A216"/>
       <c r="B216"/>
       <c r="C216"/>
@@ -15800,7 +16038,7 @@
       <c r="Y216"/>
       <c r="AC216" s="88"/>
     </row>
-    <row r="217" spans="1:29" ht="15.75">
+    <row r="217" spans="1:29" ht="16">
       <c r="A217"/>
       <c r="B217"/>
       <c r="C217"/>
@@ -15826,7 +16064,7 @@
       <c r="Y217"/>
       <c r="AC217" s="88"/>
     </row>
-    <row r="218" spans="1:29" ht="15.75">
+    <row r="218" spans="1:29" ht="16">
       <c r="A218"/>
       <c r="B218"/>
       <c r="C218"/>
@@ -15852,7 +16090,7 @@
       <c r="Y218"/>
       <c r="AC218" s="88"/>
     </row>
-    <row r="219" spans="1:29" ht="15.75">
+    <row r="219" spans="1:29" ht="16">
       <c r="A219"/>
       <c r="B219"/>
       <c r="C219"/>
@@ -15878,7 +16116,7 @@
       <c r="Y219"/>
       <c r="AC219" s="88"/>
     </row>
-    <row r="220" spans="1:29" ht="15.75">
+    <row r="220" spans="1:29" ht="16">
       <c r="A220"/>
       <c r="B220"/>
       <c r="C220"/>
@@ -15904,7 +16142,7 @@
       <c r="Y220"/>
       <c r="AC220" s="88"/>
     </row>
-    <row r="221" spans="1:29" ht="15.75">
+    <row r="221" spans="1:29" ht="16">
       <c r="A221"/>
       <c r="B221"/>
       <c r="C221"/>
@@ -15930,7 +16168,7 @@
       <c r="Y221"/>
       <c r="AC221" s="88"/>
     </row>
-    <row r="222" spans="1:29" ht="15.75">
+    <row r="222" spans="1:29" ht="16">
       <c r="A222"/>
       <c r="B222"/>
       <c r="C222"/>
@@ -15956,7 +16194,7 @@
       <c r="Y222"/>
       <c r="AC222" s="88"/>
     </row>
-    <row r="223" spans="1:29" ht="15.75">
+    <row r="223" spans="1:29" ht="16">
       <c r="A223"/>
       <c r="B223"/>
       <c r="C223"/>
@@ -15982,7 +16220,7 @@
       <c r="Y223"/>
       <c r="AC223" s="88"/>
     </row>
-    <row r="224" spans="1:29" ht="15.75">
+    <row r="224" spans="1:29" ht="16">
       <c r="A224"/>
       <c r="B224"/>
       <c r="C224"/>
@@ -16008,7 +16246,7 @@
       <c r="Y224"/>
       <c r="AC224" s="88"/>
     </row>
-    <row r="225" spans="1:29" ht="15.75">
+    <row r="225" spans="1:29" ht="16">
       <c r="A225"/>
       <c r="B225"/>
       <c r="C225"/>
@@ -16034,7 +16272,7 @@
       <c r="Y225"/>
       <c r="AC225" s="88"/>
     </row>
-    <row r="226" spans="1:29" ht="15.75">
+    <row r="226" spans="1:29" ht="16">
       <c r="A226"/>
       <c r="B226"/>
       <c r="C226"/>
@@ -16060,7 +16298,7 @@
       <c r="Y226"/>
       <c r="AC226" s="88"/>
     </row>
-    <row r="227" spans="1:29" ht="15.75">
+    <row r="227" spans="1:29" ht="16">
       <c r="A227"/>
       <c r="B227"/>
       <c r="C227"/>
@@ -16086,7 +16324,7 @@
       <c r="Y227"/>
       <c r="AC227" s="88"/>
     </row>
-    <row r="228" spans="1:29" ht="15.75">
+    <row r="228" spans="1:29" ht="16">
       <c r="A228"/>
       <c r="B228"/>
       <c r="C228"/>
@@ -16112,7 +16350,7 @@
       <c r="Y228"/>
       <c r="AC228" s="88"/>
     </row>
-    <row r="229" spans="1:29" ht="15.75">
+    <row r="229" spans="1:29" ht="16">
       <c r="A229"/>
       <c r="B229"/>
       <c r="C229"/>
@@ -16138,7 +16376,7 @@
       <c r="Y229"/>
       <c r="AC229" s="88"/>
     </row>
-    <row r="230" spans="1:29" ht="15.75">
+    <row r="230" spans="1:29" ht="16">
       <c r="A230"/>
       <c r="B230"/>
       <c r="C230"/>
@@ -16164,7 +16402,7 @@
       <c r="Y230"/>
       <c r="AC230" s="88"/>
     </row>
-    <row r="231" spans="1:29" ht="15.75">
+    <row r="231" spans="1:29" ht="16">
       <c r="A231"/>
       <c r="B231"/>
       <c r="C231"/>
@@ -16190,7 +16428,7 @@
       <c r="Y231"/>
       <c r="AC231" s="94"/>
     </row>
-    <row r="232" spans="1:29" ht="15.75">
+    <row r="232" spans="1:29" ht="16">
       <c r="A232"/>
       <c r="B232"/>
       <c r="C232"/>
@@ -16216,7 +16454,7 @@
       <c r="Y232"/>
       <c r="AC232" s="88"/>
     </row>
-    <row r="233" spans="1:29" ht="15.75">
+    <row r="233" spans="1:29" ht="16">
       <c r="A233"/>
       <c r="B233"/>
       <c r="C233"/>
@@ -16242,7 +16480,7 @@
       <c r="Y233"/>
       <c r="AC233" s="88"/>
     </row>
-    <row r="234" spans="1:29" ht="15.75">
+    <row r="234" spans="1:29" ht="16">
       <c r="A234"/>
       <c r="B234"/>
       <c r="C234"/>
@@ -16268,7 +16506,7 @@
       <c r="Y234"/>
       <c r="AC234" s="88"/>
     </row>
-    <row r="235" spans="1:29" ht="15.75">
+    <row r="235" spans="1:29" ht="16">
       <c r="A235"/>
       <c r="B235"/>
       <c r="C235"/>
@@ -16294,7 +16532,7 @@
       <c r="Y235"/>
       <c r="AC235" s="88"/>
     </row>
-    <row r="236" spans="1:29" ht="15.75">
+    <row r="236" spans="1:29" ht="16">
       <c r="A236"/>
       <c r="B236"/>
       <c r="C236"/>
@@ -16320,7 +16558,7 @@
       <c r="Y236"/>
       <c r="AC236" s="88"/>
     </row>
-    <row r="237" spans="1:29" ht="15.75">
+    <row r="237" spans="1:29" ht="16">
       <c r="A237"/>
       <c r="B237"/>
       <c r="C237"/>
@@ -16346,7 +16584,7 @@
       <c r="Y237"/>
       <c r="AC237" s="88"/>
     </row>
-    <row r="238" spans="1:29" ht="15.75">
+    <row r="238" spans="1:29" ht="16">
       <c r="A238"/>
       <c r="B238"/>
       <c r="C238"/>
@@ -16372,7 +16610,7 @@
       <c r="Y238"/>
       <c r="AC238" s="88"/>
     </row>
-    <row r="239" spans="1:29" ht="15.75">
+    <row r="239" spans="1:29" ht="16">
       <c r="A239"/>
       <c r="B239"/>
       <c r="C239"/>
@@ -16399,7 +16637,7 @@
       <c r="Z239" s="86"/>
       <c r="AC239" s="88"/>
     </row>
-    <row r="240" spans="1:29" ht="15.75">
+    <row r="240" spans="1:29" ht="16">
       <c r="A240"/>
       <c r="B240"/>
       <c r="C240"/>
@@ -16425,7 +16663,7 @@
       <c r="Y240"/>
       <c r="AC240" s="88"/>
     </row>
-    <row r="241" spans="1:29" ht="15.75">
+    <row r="241" spans="1:29" ht="16">
       <c r="A241"/>
       <c r="B241"/>
       <c r="C241"/>
@@ -16451,7 +16689,7 @@
       <c r="Y241"/>
       <c r="AC241" s="88"/>
     </row>
-    <row r="242" spans="1:29" ht="15.75">
+    <row r="242" spans="1:29" ht="16">
       <c r="A242"/>
       <c r="B242"/>
       <c r="C242"/>
@@ -16477,7 +16715,7 @@
       <c r="Y242"/>
       <c r="AC242" s="88"/>
     </row>
-    <row r="243" spans="1:29" ht="15.75">
+    <row r="243" spans="1:29" ht="16">
       <c r="A243"/>
       <c r="B243"/>
       <c r="C243"/>
@@ -16503,7 +16741,7 @@
       <c r="Y243"/>
       <c r="AC243" s="88"/>
     </row>
-    <row r="244" spans="1:29" ht="15.75">
+    <row r="244" spans="1:29" ht="16">
       <c r="A244"/>
       <c r="B244"/>
       <c r="C244"/>
@@ -16529,7 +16767,7 @@
       <c r="Y244"/>
       <c r="AC244" s="88"/>
     </row>
-    <row r="245" spans="1:29" ht="15.75">
+    <row r="245" spans="1:29" ht="16">
       <c r="A245"/>
       <c r="B245"/>
       <c r="C245"/>
@@ -16555,7 +16793,7 @@
       <c r="Y245"/>
       <c r="AC245" s="88"/>
     </row>
-    <row r="246" spans="1:29" ht="15.75">
+    <row r="246" spans="1:29" ht="16">
       <c r="A246"/>
       <c r="B246"/>
       <c r="C246"/>
@@ -16581,7 +16819,7 @@
       <c r="Y246"/>
       <c r="AC246" s="88"/>
     </row>
-    <row r="247" spans="1:29" ht="15.75">
+    <row r="247" spans="1:29" ht="16">
       <c r="A247"/>
       <c r="B247"/>
       <c r="C247"/>
@@ -16607,7 +16845,7 @@
       <c r="Y247"/>
       <c r="AC247" s="88"/>
     </row>
-    <row r="248" spans="1:29" ht="15.75">
+    <row r="248" spans="1:29" ht="16">
       <c r="A248"/>
       <c r="B248"/>
       <c r="C248"/>
@@ -16633,7 +16871,7 @@
       <c r="Y248"/>
       <c r="AC248" s="88"/>
     </row>
-    <row r="249" spans="1:29" ht="15.75">
+    <row r="249" spans="1:29" ht="16">
       <c r="A249"/>
       <c r="B249"/>
       <c r="C249"/>
@@ -16659,7 +16897,7 @@
       <c r="Y249"/>
       <c r="AC249" s="88"/>
     </row>
-    <row r="250" spans="1:29" ht="15.75">
+    <row r="250" spans="1:29" ht="16">
       <c r="A250"/>
       <c r="B250"/>
       <c r="C250"/>
@@ -16685,7 +16923,7 @@
       <c r="Y250"/>
       <c r="AC250" s="88"/>
     </row>
-    <row r="251" spans="1:29" ht="15.75">
+    <row r="251" spans="1:29" ht="16">
       <c r="A251"/>
       <c r="B251"/>
       <c r="C251"/>
@@ -16711,7 +16949,7 @@
       <c r="Y251"/>
       <c r="AC251" s="88"/>
     </row>
-    <row r="252" spans="1:29" ht="15.75">
+    <row r="252" spans="1:29" ht="16">
       <c r="A252"/>
       <c r="B252"/>
       <c r="C252"/>
@@ -16737,7 +16975,7 @@
       <c r="Y252"/>
       <c r="AC252" s="88"/>
     </row>
-    <row r="253" spans="1:29" ht="15.75">
+    <row r="253" spans="1:29" ht="16">
       <c r="A253"/>
       <c r="B253"/>
       <c r="C253"/>
@@ -16763,7 +17001,7 @@
       <c r="Y253"/>
       <c r="AC253" s="88"/>
     </row>
-    <row r="254" spans="1:29" ht="15.75">
+    <row r="254" spans="1:29" ht="16">
       <c r="A254"/>
       <c r="B254"/>
       <c r="C254"/>
@@ -16789,7 +17027,7 @@
       <c r="Y254"/>
       <c r="AC254" s="88"/>
     </row>
-    <row r="255" spans="1:29" ht="15.75">
+    <row r="255" spans="1:29" ht="16">
       <c r="A255"/>
       <c r="B255"/>
       <c r="C255"/>
@@ -16815,7 +17053,7 @@
       <c r="Y255"/>
       <c r="AC255" s="88"/>
     </row>
-    <row r="256" spans="1:29" ht="15.75">
+    <row r="256" spans="1:29" ht="16">
       <c r="A256"/>
       <c r="B256"/>
       <c r="C256"/>
@@ -16841,7 +17079,7 @@
       <c r="Y256"/>
       <c r="AC256" s="88"/>
     </row>
-    <row r="257" spans="1:29" ht="15.75">
+    <row r="257" spans="1:29" ht="16">
       <c r="A257"/>
       <c r="B257"/>
       <c r="C257"/>
@@ -16867,7 +17105,7 @@
       <c r="Y257"/>
       <c r="AC257" s="88"/>
     </row>
-    <row r="258" spans="1:29" ht="15.75">
+    <row r="258" spans="1:29" ht="16">
       <c r="A258"/>
       <c r="B258"/>
       <c r="C258"/>
@@ -16893,7 +17131,7 @@
       <c r="Y258"/>
       <c r="AC258" s="88"/>
     </row>
-    <row r="259" spans="1:29" ht="15.75">
+    <row r="259" spans="1:29" ht="16">
       <c r="A259"/>
       <c r="B259"/>
       <c r="C259"/>
@@ -18171,506 +18409,638 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC685F6-A1BF-6D48-848F-C86526624DE3}">
-  <dimension ref="A1:B120"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B60" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="92" customWidth="1"/>
+    <col min="1" max="1" width="62" style="92" customWidth="1"/>
     <col min="2" max="2" width="196" style="92" customWidth="1"/>
-    <col min="3" max="16384" width="10.85546875" style="92"/>
+    <col min="3" max="16384" width="10.81640625" style="92"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
+    <row r="1" spans="1:2" ht="18.5">
       <c r="A1" s="90"/>
       <c r="B1" s="91"/>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="111"/>
-      <c r="B2" s="93"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="112"/>
-      <c r="B3" s="93"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="112"/>
-      <c r="B4" s="93"/>
+    <row r="2" spans="1:2" ht="31">
+      <c r="A2" s="111" t="s">
+        <v>822</v>
+      </c>
+      <c r="B2" s="93" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" customHeight="1">
+      <c r="A3" s="111" t="s">
+        <v>824</v>
+      </c>
+      <c r="B3" s="89" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" customHeight="1">
+      <c r="A4" s="111" t="s">
+        <v>826</v>
+      </c>
+      <c r="B4" s="89" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="112"/>
-      <c r="B5" s="93"/>
+      <c r="A5" s="112" t="s">
+        <v>828</v>
+      </c>
+      <c r="B5" s="93" t="s">
+        <v>829</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="112"/>
-      <c r="B6" s="93"/>
+      <c r="A6" s="113"/>
+      <c r="B6" s="93" t="s">
+        <v>830</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="113"/>
-      <c r="B7" s="89"/>
-    </row>
-    <row r="8" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A8" s="111"/>
-      <c r="B8" s="89"/>
-    </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1">
-      <c r="A9" s="112"/>
-      <c r="B9" s="89"/>
-    </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1">
-      <c r="A10" s="112"/>
-      <c r="B10" s="89"/>
-    </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1">
-      <c r="A11" s="112"/>
-      <c r="B11" s="89"/>
+      <c r="A7" s="111" t="s">
+        <v>831</v>
+      </c>
+      <c r="B7" s="93" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19.5" customHeight="1">
+      <c r="A8" s="111" t="s">
+        <v>832</v>
+      </c>
+      <c r="B8" s="93" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="114" t="s">
+        <v>833</v>
+      </c>
+      <c r="B9" s="89" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="115"/>
+      <c r="B10" s="92" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="92" t="s">
+        <v>836</v>
+      </c>
+      <c r="B11" s="92" t="s">
+        <v>838</v>
+      </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="112"/>
-      <c r="B12" s="89"/>
-    </row>
-    <row r="13" spans="1:2" ht="15.95" customHeight="1">
-      <c r="A13" s="111"/>
-      <c r="B13" s="89"/>
+      <c r="A12" s="92" t="s">
+        <v>837</v>
+      </c>
+      <c r="B12" s="92" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="92" t="s">
+        <v>840</v>
+      </c>
+      <c r="B13" s="92" t="s">
+        <v>842</v>
+      </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="112"/>
-      <c r="B14" s="89"/>
+      <c r="A14" s="92" t="s">
+        <v>841</v>
+      </c>
+      <c r="B14" s="92" t="s">
+        <v>843</v>
+      </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="112"/>
-      <c r="B15" s="89"/>
+      <c r="A15" s="116" t="s">
+        <v>844</v>
+      </c>
+      <c r="B15" s="92" t="s">
+        <v>845</v>
+      </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="112"/>
-      <c r="B16" s="89"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="112"/>
-      <c r="B17" s="89"/>
+      <c r="A16" s="116"/>
+      <c r="B16" s="92" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23.5" customHeight="1">
+      <c r="A17" s="118" t="s">
+        <v>847</v>
+      </c>
+      <c r="B17" s="92" t="s">
+        <v>848</v>
+      </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="112"/>
-      <c r="B18" s="93"/>
+      <c r="A18" s="118"/>
+      <c r="B18" s="92" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="112"/>
-      <c r="B19" s="93"/>
+      <c r="A19" s="118"/>
+      <c r="B19" s="92" t="s">
+        <v>850</v>
+      </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="112"/>
-      <c r="B20" s="93"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="112"/>
-      <c r="B21" s="89"/>
+      <c r="A20" s="118"/>
+      <c r="B20" s="92" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="31">
+      <c r="A21" s="117" t="s">
+        <v>852</v>
+      </c>
+      <c r="B21" s="92" t="s">
+        <v>853</v>
+      </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="112"/>
-      <c r="B22" s="89"/>
+      <c r="A22" s="116" t="s">
+        <v>854</v>
+      </c>
+      <c r="B22" s="92" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="112"/>
-      <c r="B23" s="93"/>
+      <c r="A23" s="116"/>
+      <c r="B23" s="92" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="112"/>
-      <c r="B24" s="93"/>
+      <c r="A24" s="116"/>
+      <c r="B24" s="92" t="s">
+        <v>857</v>
+      </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="112"/>
-      <c r="B25" s="89"/>
+      <c r="A25" s="116"/>
+      <c r="B25" s="92" t="s">
+        <v>858</v>
+      </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="112"/>
-      <c r="B26" s="89"/>
+      <c r="A26" s="116"/>
+      <c r="B26" s="92" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="112"/>
-      <c r="B27" s="89"/>
+      <c r="A27" s="116"/>
+      <c r="B27" s="92" t="s">
+        <v>860</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="112"/>
-      <c r="B28" s="89"/>
+      <c r="A28" s="116"/>
+      <c r="B28" s="92" t="s">
+        <v>861</v>
+      </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="112"/>
+      <c r="A29" s="116"/>
+      <c r="B29" s="92" t="s">
+        <v>862</v>
+      </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="113"/>
-      <c r="B30" s="89"/>
+      <c r="A30" s="116"/>
+      <c r="B30" s="92" t="s">
+        <v>863</v>
+      </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="111"/>
-      <c r="B31" s="93"/>
+      <c r="A31" s="116"/>
+      <c r="B31" s="92" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="112"/>
-      <c r="B32" s="93"/>
+      <c r="A32" s="116"/>
+      <c r="B32" s="92" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="112"/>
-      <c r="B33" s="93"/>
+      <c r="A33" s="116"/>
+      <c r="B33" s="92" t="s">
+        <v>866</v>
+      </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="112"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="112"/>
-      <c r="B35" s="93"/>
+      <c r="A34" s="116"/>
+      <c r="B34" s="92" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="31" customHeight="1">
+      <c r="A35" s="118" t="s">
+        <v>868</v>
+      </c>
+      <c r="B35" s="92" t="s">
+        <v>869</v>
+      </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="112"/>
-      <c r="B36" s="93"/>
+      <c r="A36" s="118"/>
+      <c r="B36" s="92" t="s">
+        <v>870</v>
+      </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="112"/>
-      <c r="B37" s="93"/>
+      <c r="A37" s="118"/>
+      <c r="B37" s="92" t="s">
+        <v>871</v>
+      </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="112"/>
-      <c r="B38" s="93"/>
+      <c r="A38" s="118"/>
+      <c r="B38" s="92" t="s">
+        <v>872</v>
+      </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="112"/>
-      <c r="B39" s="93"/>
+      <c r="A39" s="116" t="s">
+        <v>873</v>
+      </c>
+      <c r="B39" s="92" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="112"/>
-      <c r="B40" s="89"/>
+      <c r="A40" s="116"/>
+      <c r="B40" s="92" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="112"/>
-      <c r="B41" s="89"/>
+      <c r="A41" s="116"/>
+      <c r="B41" s="92" t="s">
+        <v>857</v>
+      </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="112"/>
-      <c r="B42" s="89"/>
+      <c r="A42" s="116"/>
+      <c r="B42" s="92" t="s">
+        <v>858</v>
+      </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="112"/>
-      <c r="B43" s="89"/>
+      <c r="A43" s="116"/>
+      <c r="B43" s="92" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="112"/>
-      <c r="B44" s="89"/>
+      <c r="A44" s="116"/>
+      <c r="B44" s="92" t="s">
+        <v>860</v>
+      </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="112"/>
-      <c r="B45" s="89"/>
+      <c r="A45" s="116"/>
+      <c r="B45" s="92" t="s">
+        <v>861</v>
+      </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="112"/>
-      <c r="B46" s="89"/>
+      <c r="A46" s="116"/>
+      <c r="B46" s="92" t="s">
+        <v>862</v>
+      </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="112"/>
+      <c r="A47" s="116"/>
+      <c r="B47" s="92" t="s">
+        <v>863</v>
+      </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="113"/>
-      <c r="B48" s="89"/>
+      <c r="A48" s="116"/>
+      <c r="B48" s="92" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="111"/>
-      <c r="B49" s="89"/>
+      <c r="A49" s="116"/>
+      <c r="B49" s="92" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="113"/>
-      <c r="B50" s="89"/>
+      <c r="A50" s="116"/>
+      <c r="B50" s="92" t="s">
+        <v>866</v>
+      </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="111"/>
-      <c r="B51" s="93"/>
+      <c r="A51" s="116"/>
+      <c r="B51" s="92" t="s">
+        <v>867</v>
+      </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="112"/>
-      <c r="B52" s="93"/>
+      <c r="A52" s="116" t="s">
+        <v>874</v>
+      </c>
+      <c r="B52" s="92" t="s">
+        <v>869</v>
+      </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="112"/>
-      <c r="B53" s="93"/>
+      <c r="A53" s="116"/>
+      <c r="B53" s="92" t="s">
+        <v>870</v>
+      </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="112"/>
-      <c r="B54" s="93"/>
+      <c r="A54" s="116"/>
+      <c r="B54" s="92" t="s">
+        <v>871</v>
+      </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="112"/>
-      <c r="B55" s="93"/>
+      <c r="A55" s="116"/>
+      <c r="B55" s="92" t="s">
+        <v>872</v>
+      </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="112"/>
-      <c r="B56" s="93"/>
+      <c r="A56" s="116" t="s">
+        <v>875</v>
+      </c>
+      <c r="B56" s="92" t="s">
+        <v>848</v>
+      </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="112"/>
-      <c r="B57" s="93"/>
+      <c r="A57" s="116"/>
+      <c r="B57" s="92" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="112"/>
-      <c r="B58" s="93"/>
+      <c r="A58" s="116"/>
+      <c r="B58" s="92" t="s">
+        <v>850</v>
+      </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="112"/>
-      <c r="B59" s="93"/>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="112"/>
-      <c r="B60" s="93"/>
+      <c r="A59" s="116"/>
+      <c r="B59" s="92" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="186">
+      <c r="A60" s="117" t="s">
+        <v>876</v>
+      </c>
+      <c r="B60" s="117" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="112"/>
-      <c r="B61" s="93"/>
+      <c r="A61" s="118" t="s">
+        <v>878</v>
+      </c>
+      <c r="B61" s="92" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="112"/>
-      <c r="B62" s="93"/>
+      <c r="A62" s="118"/>
+      <c r="B62" s="92" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="112"/>
-      <c r="B63" s="93"/>
+      <c r="A63" s="118"/>
+      <c r="B63" s="92" t="s">
+        <v>857</v>
+      </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="112"/>
-      <c r="B64" s="93"/>
+      <c r="A64" s="118"/>
+      <c r="B64" s="92" t="s">
+        <v>858</v>
+      </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="112"/>
-      <c r="B65" s="93"/>
+      <c r="A65" s="118"/>
+      <c r="B65" s="92" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="112"/>
-      <c r="B66" s="93"/>
+      <c r="A66" s="118"/>
+      <c r="B66" s="92" t="s">
+        <v>860</v>
+      </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="112"/>
-      <c r="B67" s="93"/>
+      <c r="A67" s="118"/>
+      <c r="B67" s="92" t="s">
+        <v>861</v>
+      </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="112"/>
-      <c r="B68" s="89"/>
+      <c r="A68" s="118"/>
+      <c r="B68" s="92" t="s">
+        <v>862</v>
+      </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="112"/>
-      <c r="B69" s="89"/>
+      <c r="A69" s="118"/>
+      <c r="B69" s="92" t="s">
+        <v>863</v>
+      </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="112"/>
-      <c r="B70" s="89"/>
+      <c r="A70" s="118"/>
+      <c r="B70" s="92" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="112"/>
-      <c r="B71" s="89"/>
+      <c r="A71" s="118"/>
+      <c r="B71" s="92" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="112"/>
-      <c r="B72" s="93"/>
+      <c r="A72" s="118"/>
+      <c r="B72" s="92" t="s">
+        <v>866</v>
+      </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="112"/>
-      <c r="B73" s="89"/>
+      <c r="A73" s="118"/>
+      <c r="B73" s="92" t="s">
+        <v>867</v>
+      </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="112"/>
-      <c r="B74" s="89"/>
+      <c r="A74" s="118"/>
+      <c r="B74" s="92" t="s">
+        <v>879</v>
+      </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="112"/>
-      <c r="B75" s="89"/>
+      <c r="A75" s="118" t="s">
+        <v>880</v>
+      </c>
+      <c r="B75" s="92" t="s">
+        <v>869</v>
+      </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="112"/>
-      <c r="B76" s="89"/>
+      <c r="A76" s="118"/>
+      <c r="B76" s="92" t="s">
+        <v>870</v>
+      </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="112"/>
-      <c r="B77" s="89"/>
+      <c r="A77" s="118"/>
+      <c r="B77" s="92" t="s">
+        <v>871</v>
+      </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="112"/>
-      <c r="B78" s="89"/>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="112"/>
-      <c r="B79" s="89"/>
+      <c r="A78" s="118"/>
+      <c r="B78" s="92" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="31">
+      <c r="A79" s="117" t="s">
+        <v>881</v>
+      </c>
+      <c r="B79" s="92" t="s">
+        <v>882</v>
+      </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="112"/>
-      <c r="B80" s="89"/>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="112"/>
-      <c r="B81" s="89"/>
+      <c r="A80" s="117" t="s">
+        <v>883</v>
+      </c>
+      <c r="B80" s="92" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="31" customHeight="1">
+      <c r="A81" s="118" t="s">
+        <v>885</v>
+      </c>
+      <c r="B81" s="92" t="s">
+        <v>886</v>
+      </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="113"/>
-      <c r="B82" s="89"/>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="111"/>
-      <c r="B83" s="89"/>
+      <c r="A82" s="118"/>
+      <c r="B82" s="92" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="31" customHeight="1">
+      <c r="A83" s="118" t="s">
+        <v>888</v>
+      </c>
+      <c r="B83" s="92" t="s">
+        <v>838</v>
+      </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="112"/>
-      <c r="B84" s="93"/>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="112"/>
-      <c r="B85" s="93"/>
+      <c r="A84" s="118"/>
+      <c r="B84" s="92" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="31" customHeight="1">
+      <c r="A85" s="118" t="s">
+        <v>889</v>
+      </c>
+      <c r="B85" s="92" t="s">
+        <v>842</v>
+      </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="112"/>
-      <c r="B86" s="93"/>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="112"/>
-      <c r="B87" s="93"/>
+      <c r="A86" s="118"/>
+      <c r="B86" s="92" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="46.5" customHeight="1">
+      <c r="A87" s="118" t="s">
+        <v>890</v>
+      </c>
+      <c r="B87" s="92" t="s">
+        <v>891</v>
+      </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="112"/>
-      <c r="B88" s="93"/>
+      <c r="A88" s="118"/>
+      <c r="B88" s="92" t="s">
+        <v>892</v>
+      </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="112"/>
-      <c r="B89" s="89"/>
+      <c r="A89" s="118"/>
+      <c r="B89" s="92" t="s">
+        <v>893</v>
+      </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="112"/>
-      <c r="B90" s="89"/>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="113"/>
-      <c r="B91" s="89"/>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="114"/>
-      <c r="B92" s="89"/>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="115"/>
-      <c r="B93" s="89"/>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="115"/>
-      <c r="B94" s="89"/>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="115"/>
-      <c r="B95" s="89"/>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="115"/>
-      <c r="B96" s="89"/>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" s="115"/>
-      <c r="B97" s="89"/>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" s="115"/>
-      <c r="B98" s="89"/>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" s="115"/>
-      <c r="B99" s="93"/>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" s="115"/>
-      <c r="B100" s="89"/>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" s="115"/>
-      <c r="B101" s="93"/>
-    </row>
-    <row r="102" spans="1:2">
-      <c r="A102" s="115"/>
-      <c r="B102" s="93"/>
-    </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="115"/>
-      <c r="B103" s="93"/>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="115"/>
-      <c r="B104" s="89"/>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="115"/>
-      <c r="B105" s="89"/>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="115"/>
-      <c r="B106" s="93"/>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="115"/>
-      <c r="B107" s="93"/>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="115"/>
-      <c r="B108" s="89"/>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="115"/>
-      <c r="B109" s="89"/>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="115"/>
-      <c r="B110" s="89"/>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="115"/>
-      <c r="B111" s="89"/>
-    </row>
-    <row r="112" spans="1:2" ht="20.100000000000001" customHeight="1">
-      <c r="A112" s="115"/>
-      <c r="B112" s="89"/>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="115"/>
-      <c r="B113" s="89"/>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="115"/>
-      <c r="B114" s="89"/>
-    </row>
-    <row r="115" spans="1:2" ht="18" customHeight="1">
-      <c r="A115" s="115"/>
-      <c r="B115" s="89"/>
-    </row>
-    <row r="116" spans="1:2">
-      <c r="A116" s="115"/>
-      <c r="B116" s="89"/>
-    </row>
-    <row r="117" spans="1:2">
-      <c r="A117" s="115"/>
-      <c r="B117" s="89"/>
-    </row>
-    <row r="118" spans="1:2">
-      <c r="A118" s="115"/>
-      <c r="B118" s="89"/>
-    </row>
-    <row r="119" spans="1:2">
-      <c r="A119" s="115"/>
-      <c r="B119" s="89"/>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" s="116"/>
-      <c r="B120" s="89"/>
+      <c r="A90" s="118"/>
+      <c r="B90" s="92" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="46.5">
+      <c r="A91" s="117" t="s">
+        <v>895</v>
+      </c>
+      <c r="B91" s="92" t="s">
+        <v>896</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A83:A91"/>
-    <mergeCell ref="A92:A120"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A30"/>
-    <mergeCell ref="A31:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A51:A82"/>
+  <mergeCells count="15">
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A61:A74"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A22:A34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A39:A51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18685,23 +19055,23 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="29.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
-    <col min="9" max="10" width="29.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="45.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" style="2" customWidth="1"/>
-    <col min="13" max="14" width="45.42578125" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="11.453125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="29.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" style="2" customWidth="1"/>
+    <col min="9" max="10" width="29.453125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="45.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" style="2" customWidth="1"/>
+    <col min="13" max="14" width="45.453125" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="56" customFormat="1" ht="30">
+    <row r="1" spans="1:14" s="56" customFormat="1" ht="29">
       <c r="A1" s="3" t="s">
         <v>325</v>
       </c>
@@ -18777,28 +19147,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.453125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="11.453125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" style="2" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.453125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23.81640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
-    <col min="13" max="13" width="30.42578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="17" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" style="17" customWidth="1"/>
-    <col min="16" max="16" width="43.42578125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="2"/>
+    <col min="13" max="13" width="30.453125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.453125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="14.453125" style="17" customWidth="1"/>
+    <col min="16" max="16" width="43.453125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" style="2" hidden="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="56" customFormat="1" ht="30">
+    <row r="1" spans="1:17" s="56" customFormat="1" ht="29">
       <c r="A1" s="10" t="s">
         <v>802</v>
       </c>
@@ -18884,25 +19254,25 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="17" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="17" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="17" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="17" customWidth="1"/>
-    <col min="10" max="10" width="32.85546875" style="17" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="17" customWidth="1"/>
-    <col min="12" max="12" width="40.42578125" style="17" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="17" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="17"/>
+    <col min="7" max="7" width="20.453125" style="17" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" style="17" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" style="17" customWidth="1"/>
+    <col min="10" max="10" width="32.81640625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" style="17" customWidth="1"/>
+    <col min="12" max="12" width="40.453125" style="17" customWidth="1"/>
+    <col min="13" max="13" width="22.1796875" style="17" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="57" customFormat="1" ht="30">
+    <row r="1" spans="1:13" s="57" customFormat="1" ht="29">
       <c r="A1" s="60" t="s">
         <v>809</v>
       </c>
@@ -18972,31 +19342,31 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="55.42578125" style="58" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="58" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="55.453125" style="58" customWidth="1"/>
+    <col min="3" max="3" width="35.453125" style="58" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="6" width="29.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" style="58" customWidth="1"/>
+    <col min="5" max="6" width="29.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="23.453125" style="58" customWidth="1"/>
     <col min="8" max="8" width="13" style="58" customWidth="1"/>
-    <col min="9" max="9" width="55.42578125" style="58" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" style="58" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="35.42578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" style="59" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="2"/>
+    <col min="9" max="9" width="55.453125" style="58" customWidth="1"/>
+    <col min="10" max="10" width="35.453125" style="58" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="23.453125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="35.453125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="23.453125" style="59" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="56" customFormat="1" ht="30">
+    <row r="1" spans="1:14" s="56" customFormat="1" ht="29">
       <c r="A1" s="78" t="s">
         <v>815</v>
       </c>
@@ -19078,15 +19448,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B27AFAFD56B51D40A0636D2EDDB429E9" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="13d31266acc58ebd7ba55a153b38d026">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="129c8279-1928-4e9e-bf04-a22cc9c6a884" xmlns:ns3="ee7d25ce-443e-4f8a-a748-4259b6f1626e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48ed0b125055c886dae4c0216e3655b5" ns2:_="" ns3:_="">
     <xsd:import namespace="129c8279-1928-4e9e-bf04-a22cc9c6a884"/>
@@ -19315,14 +19676,49 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA070F5E-46B8-4CF5-94C0-070A58B7172E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA070F5E-46B8-4CF5-94C0-070A58B7172E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee7d25ce-443e-4f8a-a748-4259b6f1626e"/>
+    <ds:schemaRef ds:uri="129c8279-1928-4e9e-bf04-a22cc9c6a884"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B6F3CE9-A837-46EA-9FB3-9103F3863ECD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80AF805D-BBAB-438F-A2B3-36BD6E56A636}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="129c8279-1928-4e9e-bf04-a22cc9c6a884"/>
+    <ds:schemaRef ds:uri="ee7d25ce-443e-4f8a-a748-4259b6f1626e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80AF805D-BBAB-438F-A2B3-36BD6E56A636}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B6F3CE9-A837-46EA-9FB3-9103F3863ECD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>